<commit_message>
remove one arm from a study
</commit_message>
<xml_diff>
--- a/hexa_review.xlsx
+++ b/hexa_review.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://bmgf-my.sharepoint.com/personal/qifang_bi_gatesfoundation_org/Documents/Hexa/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://bmgf-my.sharepoint.com/personal/qifang_bi_gatesfoundation_org/Documents/Repository/hexa_dosing/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="2004" documentId="8_{3E1959A5-03D9-489A-814E-73E2A90AC25F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{49297956-028F-400A-B4C0-CEAFBB06ABC0}"/>
+  <xr:revisionPtr revIDLastSave="2112" documentId="8_{3E1959A5-03D9-489A-814E-73E2A90AC25F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{71CBB789-CB68-460F-A8A1-B9FF66E8ACF9}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11620" xr2:uid="{6686FE0B-19D2-4DD2-8D2B-E91F6EF7CA1A}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11620" activeTab="2" xr2:uid="{6686FE0B-19D2-4DD2-8D2B-E91F6EF7CA1A}"/>
   </bookViews>
   <sheets>
     <sheet name="readme" sheetId="5" r:id="rId1"/>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2902" uniqueCount="1451">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2886" uniqueCount="1470">
   <si>
     <t>PMID</t>
   </si>
@@ -4395,24 +4395,9 @@
     <t>Philippines</t>
   </si>
   <si>
-    <t>correct</t>
-  </si>
-  <si>
-    <t>correct but check strain</t>
-  </si>
-  <si>
     <t>IPV by Sanofi</t>
   </si>
   <si>
-    <t>3 doses now</t>
-  </si>
-  <si>
-    <t>no longer included in analysis</t>
-  </si>
-  <si>
-    <t>March3correction</t>
-  </si>
-  <si>
     <t>EasySix</t>
   </si>
   <si>
@@ -4450,6 +4435,81 @@
   </si>
   <si>
     <t>ipv pubmed pull</t>
+  </si>
+  <si>
+    <t>neutralizing_antibody_against</t>
+  </si>
+  <si>
+    <t>sabin</t>
+  </si>
+  <si>
+    <t>unclear</t>
+  </si>
+  <si>
+    <t>referenced https://link.springer.com/protocol/10.1007/978-1-4939-3292-4_8</t>
+  </si>
+  <si>
+    <t>Neutralization antibodies
+against poliovirus types 1, 2, and 3</t>
+  </si>
+  <si>
+    <t>referenced https://link.springer.com/protocol/10.1007/978-1-4939-3292-4_9</t>
+  </si>
+  <si>
+    <t>referenced https://link.springer.com/protocol/10.1007/978-1-4939-3292-4_10</t>
+  </si>
+  <si>
+    <t>referenced https://link.springer.com/protocol/10.1007/978-1-4939-3292-4_11</t>
+  </si>
+  <si>
+    <t>referenced https://link.springer.com/protocol/10.1007/978-1-4939-3292-4_12</t>
+  </si>
+  <si>
+    <t>referenced https://link.springer.com/protocol/10.1007/978-1-4939-3292-4_13</t>
+  </si>
+  <si>
+    <t>referenced https://link.springer.com/protocol/10.1007/978-1-4939-3292-4_14</t>
+  </si>
+  <si>
+    <t>referenced https://link.springer.com/protocol/10.1007/978-1-4939-3292-4_15</t>
+  </si>
+  <si>
+    <t>referenced https://link.springer.com/protocol/10.1007/978-1-4939-3292-4_16</t>
+  </si>
+  <si>
+    <t>unspecified</t>
+  </si>
+  <si>
+    <t>study not included</t>
+  </si>
+  <si>
+    <t>sabin or wild type</t>
+  </si>
+  <si>
+    <t>unspecified "neutralising antibodies against poliovirus types 1, 2, and 3"</t>
+  </si>
+  <si>
+    <t>unspecified "neutralizing antibodies against poliovirus 1, 2, and 3"</t>
+  </si>
+  <si>
+    <t>unspecified "neutralising antibodies against polioviruses type 1, type 2, and type 3"</t>
+  </si>
+  <si>
+    <t>unspecified "The polio microneutralization assay was used to measure
+antibody titers to poliovirus 1, 2, and 3"</t>
+  </si>
+  <si>
+    <t>unspecified "modified neutralization assays for antibodies to types
+1, 2, and 3 poliovirus"</t>
+  </si>
+  <si>
+    <t>unspecified  "(nAb) seroconversion percentages for poliovirus types 1, 2, and 3."</t>
+  </si>
+  <si>
+    <t>unspecified "neutralizing antibody titres against poliovirus types 1, 2, and 3"</t>
+  </si>
+  <si>
+    <t>unspecified "Serum samples were collected fromall infants before and 30 days after vaccination with 3 doses of each vaccine for detection of anti–poliovirus-neutralizing antibodies."</t>
   </si>
 </sst>
 </file>
@@ -5000,7 +5060,7 @@
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -5035,15 +5095,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="42"/>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="42" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="26" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="42" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="43">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -5422,7 +5481,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{08054094-7407-4096-8757-273A09F30234}">
   <dimension ref="A1:B5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F27" sqref="F27"/>
     </sheetView>
   </sheetViews>
@@ -5433,42 +5492,42 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" t="s">
-        <v>1441</v>
+        <v>1436</v>
       </c>
       <c r="B1" t="s">
-        <v>1442</v>
+        <v>1437</v>
       </c>
     </row>
     <row r="2" spans="1:2">
       <c r="A2" t="s">
-        <v>1443</v>
+        <v>1438</v>
       </c>
       <c r="B2" t="s">
-        <v>1444</v>
+        <v>1439</v>
       </c>
     </row>
     <row r="3" spans="1:2">
       <c r="A3" t="s">
-        <v>1445</v>
+        <v>1440</v>
       </c>
       <c r="B3" t="s">
-        <v>1446</v>
+        <v>1441</v>
       </c>
     </row>
     <row r="4" spans="1:2">
       <c r="A4" t="s">
-        <v>1447</v>
+        <v>1442</v>
       </c>
       <c r="B4" t="s">
-        <v>1448</v>
+        <v>1443</v>
       </c>
     </row>
     <row r="5" spans="1:2">
       <c r="A5" t="s">
-        <v>1450</v>
+        <v>1445</v>
       </c>
       <c r="B5" t="s">
-        <v>1449</v>
+        <v>1444</v>
       </c>
     </row>
   </sheetData>
@@ -5480,8 +5539,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BCECA026-A481-4661-B5E1-656ABE78B0F5}">
   <dimension ref="A1:W1048575"/>
   <sheetViews>
-    <sheetView topLeftCell="A51" zoomScale="91" workbookViewId="0">
-      <selection activeCell="C92" sqref="C92"/>
+    <sheetView topLeftCell="A8" zoomScale="91" workbookViewId="0">
+      <selection activeCell="I21" sqref="I21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -5522,7 +5581,7 @@
         <v>6</v>
       </c>
       <c r="I1" t="s">
-        <v>1437</v>
+        <v>1446</v>
       </c>
       <c r="J1" t="s">
         <v>7</v>
@@ -5581,9 +5640,6 @@
       <c r="H2">
         <v>4</v>
       </c>
-      <c r="I2" t="s">
-        <v>1432</v>
-      </c>
       <c r="J2" t="s">
         <v>21</v>
       </c>
@@ -5634,9 +5690,6 @@
       <c r="H3">
         <v>4</v>
       </c>
-      <c r="I3" t="s">
-        <v>1432</v>
-      </c>
       <c r="J3" t="s">
         <v>21</v>
       </c>
@@ -5687,9 +5740,6 @@
       <c r="H4">
         <v>4</v>
       </c>
-      <c r="I4" t="s">
-        <v>1432</v>
-      </c>
       <c r="J4" t="s">
         <v>21</v>
       </c>
@@ -5741,7 +5791,7 @@
         <v>3</v>
       </c>
       <c r="I5" t="s">
-        <v>1433</v>
+        <v>1447</v>
       </c>
       <c r="J5" t="s">
         <v>21</v>
@@ -5797,7 +5847,7 @@
         <v>3</v>
       </c>
       <c r="I6" t="s">
-        <v>1433</v>
+        <v>1447</v>
       </c>
       <c r="J6" t="s">
         <v>21</v>
@@ -5853,7 +5903,7 @@
         <v>3</v>
       </c>
       <c r="I7" t="s">
-        <v>1433</v>
+        <v>1447</v>
       </c>
       <c r="J7" t="s">
         <v>21</v>
@@ -5909,7 +5959,7 @@
         <v>3</v>
       </c>
       <c r="I8" t="s">
-        <v>1433</v>
+        <v>28</v>
       </c>
       <c r="J8" t="s">
         <v>21</v>
@@ -5965,7 +6015,7 @@
         <v>3</v>
       </c>
       <c r="I9" t="s">
-        <v>1433</v>
+        <v>28</v>
       </c>
       <c r="J9" t="s">
         <v>21</v>
@@ -6021,7 +6071,7 @@
         <v>3</v>
       </c>
       <c r="I10" t="s">
-        <v>1433</v>
+        <v>28</v>
       </c>
       <c r="J10" t="s">
         <v>21</v>
@@ -6077,7 +6127,7 @@
         <v>3</v>
       </c>
       <c r="I11" t="s">
-        <v>1433</v>
+        <v>1447</v>
       </c>
       <c r="J11" t="s">
         <v>29</v>
@@ -6133,7 +6183,7 @@
         <v>3</v>
       </c>
       <c r="I12" t="s">
-        <v>1433</v>
+        <v>1447</v>
       </c>
       <c r="J12" t="s">
         <v>29</v>
@@ -6189,7 +6239,7 @@
         <v>3</v>
       </c>
       <c r="I13" t="s">
-        <v>1433</v>
+        <v>1447</v>
       </c>
       <c r="J13" t="s">
         <v>29</v>
@@ -6245,7 +6295,7 @@
         <v>3</v>
       </c>
       <c r="I14" t="s">
-        <v>1433</v>
+        <v>28</v>
       </c>
       <c r="J14" t="s">
         <v>29</v>
@@ -6301,7 +6351,7 @@
         <v>3</v>
       </c>
       <c r="I15" t="s">
-        <v>1433</v>
+        <v>28</v>
       </c>
       <c r="J15" t="s">
         <v>29</v>
@@ -6357,7 +6407,7 @@
         <v>3</v>
       </c>
       <c r="I16" t="s">
-        <v>1433</v>
+        <v>28</v>
       </c>
       <c r="J16" t="s">
         <v>29</v>
@@ -6413,7 +6463,7 @@
         <v>2</v>
       </c>
       <c r="I17" t="s">
-        <v>23</v>
+        <v>1449</v>
       </c>
       <c r="J17" t="s">
         <v>29</v>
@@ -6466,7 +6516,7 @@
         <v>2</v>
       </c>
       <c r="I18" t="s">
-        <v>23</v>
+        <v>1451</v>
       </c>
       <c r="J18" t="s">
         <v>29</v>
@@ -6519,7 +6569,7 @@
         <v>2</v>
       </c>
       <c r="I19" t="s">
-        <v>23</v>
+        <v>1452</v>
       </c>
       <c r="J19" t="s">
         <v>29</v>
@@ -6572,7 +6622,7 @@
         <v>2</v>
       </c>
       <c r="I20" t="s">
-        <v>23</v>
+        <v>1453</v>
       </c>
       <c r="J20" t="s">
         <v>29</v>
@@ -6625,7 +6675,7 @@
         <v>2</v>
       </c>
       <c r="I21" t="s">
-        <v>23</v>
+        <v>1454</v>
       </c>
       <c r="J21" t="s">
         <v>29</v>
@@ -6678,7 +6728,7 @@
         <v>2</v>
       </c>
       <c r="I22" t="s">
-        <v>23</v>
+        <v>1455</v>
       </c>
       <c r="J22" t="s">
         <v>29</v>
@@ -6731,7 +6781,7 @@
         <v>2</v>
       </c>
       <c r="I23" t="s">
-        <v>23</v>
+        <v>1456</v>
       </c>
       <c r="J23" t="s">
         <v>29</v>
@@ -6784,7 +6834,7 @@
         <v>2</v>
       </c>
       <c r="I24" t="s">
-        <v>23</v>
+        <v>1457</v>
       </c>
       <c r="J24" t="s">
         <v>29</v>
@@ -6837,7 +6887,7 @@
         <v>2</v>
       </c>
       <c r="I25" t="s">
-        <v>23</v>
+        <v>1458</v>
       </c>
       <c r="J25" t="s">
         <v>29</v>
@@ -6889,9 +6939,6 @@
       <c r="H26">
         <v>3</v>
       </c>
-      <c r="I26" t="s">
-        <v>23</v>
-      </c>
       <c r="J26" t="s">
         <v>21</v>
       </c>
@@ -6945,9 +6992,6 @@
       <c r="H27">
         <v>3</v>
       </c>
-      <c r="I27" t="s">
-        <v>23</v>
-      </c>
       <c r="J27" t="s">
         <v>21</v>
       </c>
@@ -7001,9 +7045,6 @@
       <c r="H28">
         <v>3</v>
       </c>
-      <c r="I28" t="s">
-        <v>23</v>
-      </c>
       <c r="J28" t="s">
         <v>21</v>
       </c>
@@ -7057,9 +7098,6 @@
       <c r="H29">
         <v>3</v>
       </c>
-      <c r="I29" t="s">
-        <v>23</v>
-      </c>
       <c r="J29" t="s">
         <v>21</v>
       </c>
@@ -7113,9 +7151,6 @@
       <c r="H30">
         <v>3</v>
       </c>
-      <c r="I30" t="s">
-        <v>23</v>
-      </c>
       <c r="J30" t="s">
         <v>21</v>
       </c>
@@ -7169,9 +7204,6 @@
       <c r="H31">
         <v>3</v>
       </c>
-      <c r="I31" t="s">
-        <v>23</v>
-      </c>
       <c r="J31" t="s">
         <v>21</v>
       </c>
@@ -7200,7 +7232,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="32" spans="1:19">
+    <row r="32" spans="1:19" ht="58">
       <c r="A32">
         <v>106</v>
       </c>
@@ -7225,8 +7257,8 @@
       <c r="H32">
         <v>3</v>
       </c>
-      <c r="I32" t="s">
-        <v>1432</v>
+      <c r="I32" s="13" t="s">
+        <v>1450</v>
       </c>
       <c r="J32" t="s">
         <v>43</v>
@@ -7279,9 +7311,6 @@
       <c r="H33">
         <v>3</v>
       </c>
-      <c r="I33" t="s">
-        <v>1432</v>
-      </c>
       <c r="J33" t="s">
         <v>43</v>
       </c>
@@ -7333,9 +7362,6 @@
       <c r="H34">
         <v>3</v>
       </c>
-      <c r="I34" t="s">
-        <v>1432</v>
-      </c>
       <c r="J34" t="s">
         <v>43</v>
       </c>
@@ -7387,14 +7413,11 @@
       <c r="H35">
         <v>3</v>
       </c>
-      <c r="I35" t="s">
-        <v>1432</v>
-      </c>
       <c r="J35" t="s">
         <v>29</v>
       </c>
       <c r="K35" t="s">
-        <v>1434</v>
+        <v>1432</v>
       </c>
       <c r="M35">
         <v>1</v>
@@ -7441,14 +7464,11 @@
       <c r="H36">
         <v>3</v>
       </c>
-      <c r="I36" t="s">
-        <v>1432</v>
-      </c>
       <c r="J36" t="s">
         <v>29</v>
       </c>
       <c r="K36" t="s">
-        <v>1434</v>
+        <v>1432</v>
       </c>
       <c r="M36">
         <v>2</v>
@@ -7495,14 +7515,11 @@
       <c r="H37">
         <v>3</v>
       </c>
-      <c r="I37" t="s">
-        <v>1432</v>
-      </c>
       <c r="J37" t="s">
         <v>29</v>
       </c>
       <c r="K37" t="s">
-        <v>1434</v>
+        <v>1432</v>
       </c>
       <c r="M37">
         <v>3</v>
@@ -7550,7 +7567,7 @@
         <v>3</v>
       </c>
       <c r="I38" t="s">
-        <v>1432</v>
+        <v>1447</v>
       </c>
       <c r="J38" t="s">
         <v>21</v>
@@ -7603,7 +7620,7 @@
         <v>3</v>
       </c>
       <c r="I39" t="s">
-        <v>1432</v>
+        <v>1447</v>
       </c>
       <c r="J39" t="s">
         <v>29</v>
@@ -7656,7 +7673,7 @@
         <v>3</v>
       </c>
       <c r="I40" t="s">
-        <v>1432</v>
+        <v>1447</v>
       </c>
       <c r="J40" t="s">
         <v>21</v>
@@ -7709,7 +7726,7 @@
         <v>3</v>
       </c>
       <c r="I41" t="s">
-        <v>1432</v>
+        <v>1447</v>
       </c>
       <c r="J41" t="s">
         <v>21</v>
@@ -7762,7 +7779,7 @@
         <v>3</v>
       </c>
       <c r="I42" t="s">
-        <v>1432</v>
+        <v>1447</v>
       </c>
       <c r="J42" t="s">
         <v>29</v>
@@ -7815,7 +7832,7 @@
         <v>3</v>
       </c>
       <c r="I43" t="s">
-        <v>1432</v>
+        <v>1447</v>
       </c>
       <c r="J43" t="s">
         <v>21</v>
@@ -7868,7 +7885,7 @@
         <v>3</v>
       </c>
       <c r="I44" t="s">
-        <v>1432</v>
+        <v>1447</v>
       </c>
       <c r="J44" t="s">
         <v>21</v>
@@ -7921,7 +7938,7 @@
         <v>3</v>
       </c>
       <c r="I45" t="s">
-        <v>1432</v>
+        <v>1447</v>
       </c>
       <c r="J45" t="s">
         <v>29</v>
@@ -7974,7 +7991,7 @@
         <v>3</v>
       </c>
       <c r="I46" t="s">
-        <v>1432</v>
+        <v>1447</v>
       </c>
       <c r="J46" t="s">
         <v>21</v>
@@ -8027,7 +8044,7 @@
         <v>3</v>
       </c>
       <c r="I47" t="s">
-        <v>1432</v>
+        <v>1447</v>
       </c>
       <c r="J47" t="s">
         <v>29</v>
@@ -8083,7 +8100,7 @@
         <v>3</v>
       </c>
       <c r="I48" t="s">
-        <v>1432</v>
+        <v>1447</v>
       </c>
       <c r="J48" t="s">
         <v>29</v>
@@ -8139,7 +8156,7 @@
         <v>3</v>
       </c>
       <c r="I49" t="s">
-        <v>1432</v>
+        <v>1447</v>
       </c>
       <c r="J49" t="s">
         <v>29</v>
@@ -8195,7 +8212,7 @@
         <v>3</v>
       </c>
       <c r="I50" t="s">
-        <v>1432</v>
+        <v>1447</v>
       </c>
       <c r="J50" t="s">
         <v>29</v>
@@ -8251,7 +8268,7 @@
         <v>3</v>
       </c>
       <c r="I51" t="s">
-        <v>1432</v>
+        <v>1447</v>
       </c>
       <c r="J51" t="s">
         <v>29</v>
@@ -8307,7 +8324,7 @@
         <v>3</v>
       </c>
       <c r="I52" t="s">
-        <v>1432</v>
+        <v>1447</v>
       </c>
       <c r="J52" t="s">
         <v>29</v>
@@ -8363,7 +8380,7 @@
         <v>3</v>
       </c>
       <c r="I53" t="s">
-        <v>1432</v>
+        <v>1447</v>
       </c>
       <c r="J53" t="s">
         <v>29</v>
@@ -8419,7 +8436,7 @@
         <v>3</v>
       </c>
       <c r="I54" t="s">
-        <v>1432</v>
+        <v>1447</v>
       </c>
       <c r="J54" t="s">
         <v>29</v>
@@ -8474,9 +8491,6 @@
       <c r="H55">
         <v>3</v>
       </c>
-      <c r="I55" t="s">
-        <v>1432</v>
-      </c>
       <c r="J55" t="s">
         <v>29</v>
       </c>
@@ -8530,9 +8544,6 @@
       <c r="H56">
         <v>3</v>
       </c>
-      <c r="I56" t="s">
-        <v>23</v>
-      </c>
       <c r="J56" t="s">
         <v>57</v>
       </c>
@@ -8586,9 +8597,6 @@
       <c r="H57">
         <v>3</v>
       </c>
-      <c r="I57" t="s">
-        <v>23</v>
-      </c>
       <c r="J57" t="s">
         <v>57</v>
       </c>
@@ -8642,9 +8650,6 @@
       <c r="H58">
         <v>3</v>
       </c>
-      <c r="I58" t="s">
-        <v>23</v>
-      </c>
       <c r="J58" t="s">
         <v>57</v>
       </c>
@@ -8698,9 +8703,6 @@
       <c r="H59">
         <v>3</v>
       </c>
-      <c r="I59" t="s">
-        <v>23</v>
-      </c>
       <c r="J59" t="s">
         <v>57</v>
       </c>
@@ -8754,9 +8756,6 @@
       <c r="H60">
         <v>3</v>
       </c>
-      <c r="I60" t="s">
-        <v>23</v>
-      </c>
       <c r="J60" t="s">
         <v>57</v>
       </c>
@@ -8810,9 +8809,6 @@
       <c r="H61">
         <v>3</v>
       </c>
-      <c r="I61" t="s">
-        <v>23</v>
-      </c>
       <c r="J61" t="s">
         <v>57</v>
       </c>
@@ -8866,10 +8862,8 @@
       <c r="H62">
         <v>3</v>
       </c>
-      <c r="I62" s="19" t="s">
-        <v>21</v>
-      </c>
-      <c r="J62" s="19" t="s">
+      <c r="I62" s="14"/>
+      <c r="J62" s="14" t="s">
         <v>21</v>
       </c>
       <c r="K62" t="s">
@@ -8922,10 +8916,8 @@
       <c r="H63">
         <v>3</v>
       </c>
-      <c r="I63" s="19" t="s">
-        <v>21</v>
-      </c>
-      <c r="J63" s="19" t="s">
+      <c r="I63" s="14"/>
+      <c r="J63" s="14" t="s">
         <v>21</v>
       </c>
       <c r="K63" t="s">
@@ -8978,10 +8970,8 @@
       <c r="H64">
         <v>3</v>
       </c>
-      <c r="I64" s="19" t="s">
-        <v>21</v>
-      </c>
-      <c r="J64" s="19" t="s">
+      <c r="I64" s="14"/>
+      <c r="J64" s="14" t="s">
         <v>21</v>
       </c>
       <c r="K64" t="s">
@@ -9034,10 +9024,8 @@
       <c r="H65">
         <v>3</v>
       </c>
-      <c r="I65" s="19" t="s">
-        <v>21</v>
-      </c>
-      <c r="J65" s="19" t="s">
+      <c r="I65" s="14"/>
+      <c r="J65" s="14" t="s">
         <v>21</v>
       </c>
       <c r="K65" t="s">
@@ -9090,10 +9078,8 @@
       <c r="H66">
         <v>3</v>
       </c>
-      <c r="I66" s="19" t="s">
-        <v>21</v>
-      </c>
-      <c r="J66" s="19" t="s">
+      <c r="I66" s="14"/>
+      <c r="J66" s="14" t="s">
         <v>21</v>
       </c>
       <c r="K66" t="s">
@@ -9146,10 +9132,8 @@
       <c r="H67">
         <v>3</v>
       </c>
-      <c r="I67" s="19" t="s">
-        <v>21</v>
-      </c>
-      <c r="J67" s="19" t="s">
+      <c r="I67" s="14"/>
+      <c r="J67" s="14" t="s">
         <v>21</v>
       </c>
       <c r="K67" t="s">
@@ -9202,14 +9186,14 @@
       <c r="H68">
         <v>3</v>
       </c>
-      <c r="I68" s="19" t="s">
-        <v>1432</v>
+      <c r="I68" s="14" t="s">
+        <v>1447</v>
       </c>
       <c r="J68" t="s">
-        <v>1440</v>
+        <v>1435</v>
       </c>
       <c r="K68" t="s">
-        <v>1439</v>
+        <v>1434</v>
       </c>
       <c r="M68">
         <v>1</v>
@@ -9255,14 +9239,14 @@
       <c r="H69">
         <v>3</v>
       </c>
-      <c r="I69" s="19" t="s">
-        <v>1432</v>
+      <c r="I69" s="14" t="s">
+        <v>1447</v>
       </c>
       <c r="J69" t="s">
-        <v>1440</v>
+        <v>1435</v>
       </c>
       <c r="K69" t="s">
-        <v>1439</v>
+        <v>1434</v>
       </c>
       <c r="M69">
         <v>2</v>
@@ -9308,14 +9292,14 @@
       <c r="H70">
         <v>3</v>
       </c>
-      <c r="I70" s="19" t="s">
-        <v>1432</v>
+      <c r="I70" s="14" t="s">
+        <v>1447</v>
       </c>
       <c r="J70" t="s">
-        <v>1440</v>
+        <v>1435</v>
       </c>
       <c r="K70" t="s">
-        <v>1439</v>
+        <v>1434</v>
       </c>
       <c r="M70">
         <v>3</v>
@@ -9361,8 +9345,8 @@
       <c r="H71">
         <v>3</v>
       </c>
-      <c r="I71" s="19" t="s">
-        <v>1432</v>
+      <c r="I71" s="14" t="s">
+        <v>1447</v>
       </c>
       <c r="J71" t="s">
         <v>29</v>
@@ -9414,8 +9398,8 @@
       <c r="H72">
         <v>3</v>
       </c>
-      <c r="I72" s="19" t="s">
-        <v>1432</v>
+      <c r="I72" s="14" t="s">
+        <v>1447</v>
       </c>
       <c r="J72" t="s">
         <v>29</v>
@@ -9467,8 +9451,8 @@
       <c r="H73">
         <v>3</v>
       </c>
-      <c r="I73" s="19" t="s">
-        <v>1432</v>
+      <c r="I73" s="14" t="s">
+        <v>1447</v>
       </c>
       <c r="J73" t="s">
         <v>29</v>
@@ -9520,14 +9504,14 @@
       <c r="H74">
         <v>3</v>
       </c>
-      <c r="I74" s="19" t="s">
-        <v>1432</v>
+      <c r="I74" s="14" t="s">
+        <v>1448</v>
       </c>
       <c r="J74" t="s">
-        <v>1440</v>
+        <v>1435</v>
       </c>
       <c r="K74" t="s">
-        <v>1438</v>
+        <v>1433</v>
       </c>
       <c r="M74">
         <v>1</v>
@@ -9573,14 +9557,14 @@
       <c r="H75">
         <v>3</v>
       </c>
-      <c r="I75" s="19" t="s">
-        <v>1432</v>
+      <c r="I75" s="14" t="s">
+        <v>1448</v>
       </c>
       <c r="J75" t="s">
-        <v>1440</v>
+        <v>1435</v>
       </c>
       <c r="K75" t="s">
-        <v>1438</v>
+        <v>1433</v>
       </c>
       <c r="M75">
         <v>2</v>
@@ -9626,14 +9610,14 @@
       <c r="H76">
         <v>3</v>
       </c>
-      <c r="I76" s="19" t="s">
-        <v>1432</v>
+      <c r="I76" s="14" t="s">
+        <v>1448</v>
       </c>
       <c r="J76" t="s">
-        <v>1440</v>
+        <v>1435</v>
       </c>
       <c r="K76" t="s">
-        <v>1438</v>
+        <v>1433</v>
       </c>
       <c r="M76">
         <v>3</v>
@@ -9679,8 +9663,8 @@
       <c r="H77">
         <v>3</v>
       </c>
-      <c r="I77" s="19" t="s">
-        <v>1432</v>
+      <c r="I77" s="14" t="s">
+        <v>1448</v>
       </c>
       <c r="J77" t="s">
         <v>29</v>
@@ -9732,8 +9716,8 @@
       <c r="H78">
         <v>3</v>
       </c>
-      <c r="I78" s="19" t="s">
-        <v>1432</v>
+      <c r="I78" s="14" t="s">
+        <v>1448</v>
       </c>
       <c r="J78" t="s">
         <v>29</v>
@@ -9785,8 +9769,8 @@
       <c r="H79">
         <v>3</v>
       </c>
-      <c r="I79" s="19" t="s">
-        <v>1432</v>
+      <c r="I79" s="14" t="s">
+        <v>1448</v>
       </c>
       <c r="J79" t="s">
         <v>29</v>
@@ -9820,7 +9804,7 @@
       <c r="B80" t="s">
         <v>71</v>
       </c>
-      <c r="C80" s="19" t="s">
+      <c r="C80" s="14" t="s">
         <v>72</v>
       </c>
       <c r="D80" s="3" t="s">
@@ -9838,11 +9822,9 @@
       <c r="H80">
         <v>3</v>
       </c>
-      <c r="I80" s="19" t="s">
+      <c r="I80" s="14"/>
+      <c r="J80" t="s">
         <v>1435</v>
-      </c>
-      <c r="J80" t="s">
-        <v>1440</v>
       </c>
       <c r="K80" t="s">
         <v>76</v>
@@ -9876,7 +9858,7 @@
       <c r="B81" t="s">
         <v>71</v>
       </c>
-      <c r="C81" s="19" t="s">
+      <c r="C81" s="14" t="s">
         <v>72</v>
       </c>
       <c r="D81" s="3" t="s">
@@ -9894,11 +9876,9 @@
       <c r="H81">
         <v>3</v>
       </c>
-      <c r="I81" s="19" t="s">
+      <c r="I81" s="14"/>
+      <c r="J81" t="s">
         <v>1435</v>
-      </c>
-      <c r="J81" t="s">
-        <v>1440</v>
       </c>
       <c r="K81" t="s">
         <v>76</v>
@@ -9932,7 +9912,7 @@
       <c r="B82" t="s">
         <v>71</v>
       </c>
-      <c r="C82" s="19" t="s">
+      <c r="C82" s="14" t="s">
         <v>72</v>
       </c>
       <c r="D82" s="3" t="s">
@@ -9950,11 +9930,9 @@
       <c r="H82">
         <v>3</v>
       </c>
-      <c r="I82" s="19" t="s">
+      <c r="I82" s="14"/>
+      <c r="J82" t="s">
         <v>1435</v>
-      </c>
-      <c r="J82" t="s">
-        <v>1440</v>
       </c>
       <c r="K82" t="s">
         <v>76</v>
@@ -9988,7 +9966,7 @@
       <c r="B83" t="s">
         <v>71</v>
       </c>
-      <c r="C83" s="19" t="s">
+      <c r="C83" s="14" t="s">
         <v>72</v>
       </c>
       <c r="D83" s="3" t="s">
@@ -10006,9 +9984,7 @@
       <c r="H83">
         <v>3</v>
       </c>
-      <c r="I83" s="19" t="s">
-        <v>1436</v>
-      </c>
+      <c r="I83" s="14"/>
       <c r="J83" t="s">
         <v>77</v>
       </c>
@@ -10044,7 +10020,7 @@
       <c r="B84" t="s">
         <v>71</v>
       </c>
-      <c r="C84" s="19" t="s">
+      <c r="C84" s="14" t="s">
         <v>72</v>
       </c>
       <c r="D84" s="3" t="s">
@@ -10062,9 +10038,7 @@
       <c r="H84">
         <v>3</v>
       </c>
-      <c r="I84" s="19" t="s">
-        <v>1436</v>
-      </c>
+      <c r="I84" s="14"/>
       <c r="J84" t="s">
         <v>77</v>
       </c>
@@ -10100,7 +10074,7 @@
       <c r="B85" t="s">
         <v>71</v>
       </c>
-      <c r="C85" s="19" t="s">
+      <c r="C85" s="14" t="s">
         <v>72</v>
       </c>
       <c r="D85" s="3" t="s">
@@ -10118,9 +10092,7 @@
       <c r="H85">
         <v>3</v>
       </c>
-      <c r="I85" s="19" t="s">
-        <v>1436</v>
-      </c>
+      <c r="I85" s="14"/>
       <c r="J85" t="s">
         <v>77</v>
       </c>
@@ -10171,10 +10143,10 @@
       <c r="H86">
         <v>4</v>
       </c>
-      <c r="I86" s="19" t="s">
-        <v>1432</v>
-      </c>
-      <c r="J86" s="19" t="s">
+      <c r="I86" s="14" t="s">
+        <v>1447</v>
+      </c>
+      <c r="J86" s="14" t="s">
         <v>29</v>
       </c>
       <c r="K86" t="s">
@@ -10221,10 +10193,10 @@
       <c r="H87">
         <v>4</v>
       </c>
-      <c r="I87" s="19" t="s">
-        <v>1432</v>
-      </c>
-      <c r="J87" s="19" t="s">
+      <c r="I87" s="14" t="s">
+        <v>1447</v>
+      </c>
+      <c r="J87" s="14" t="s">
         <v>29</v>
       </c>
       <c r="K87" t="s">
@@ -10271,10 +10243,10 @@
       <c r="H88">
         <v>4</v>
       </c>
-      <c r="I88" s="19" t="s">
-        <v>1432</v>
-      </c>
-      <c r="J88" s="19" t="s">
+      <c r="I88" s="14" t="s">
+        <v>1447</v>
+      </c>
+      <c r="J88" s="14" t="s">
         <v>29</v>
       </c>
       <c r="K88" t="s">
@@ -10321,8 +10293,8 @@
       <c r="H89">
         <v>4</v>
       </c>
-      <c r="I89" s="19" t="s">
-        <v>1432</v>
+      <c r="I89" s="14" t="s">
+        <v>1447</v>
       </c>
       <c r="J89" t="s">
         <v>21</v>
@@ -10371,8 +10343,8 @@
       <c r="H90">
         <v>4</v>
       </c>
-      <c r="I90" s="19" t="s">
-        <v>1432</v>
+      <c r="I90" s="14" t="s">
+        <v>1447</v>
       </c>
       <c r="J90" t="s">
         <v>21</v>
@@ -10421,8 +10393,8 @@
       <c r="H91">
         <v>4</v>
       </c>
-      <c r="I91" s="19" t="s">
-        <v>1432</v>
+      <c r="I91" s="14" t="s">
+        <v>1447</v>
       </c>
       <c r="J91" t="s">
         <v>21</v>
@@ -10471,9 +10443,7 @@
       <c r="H92">
         <v>3</v>
       </c>
-      <c r="I92" s="19" t="s">
-        <v>1432</v>
-      </c>
+      <c r="I92" s="14"/>
       <c r="J92" t="s">
         <v>21</v>
       </c>
@@ -10521,9 +10491,7 @@
       <c r="H93">
         <v>3</v>
       </c>
-      <c r="I93" s="19" t="s">
-        <v>1432</v>
-      </c>
+      <c r="I93" s="14"/>
       <c r="J93" t="s">
         <v>21</v>
       </c>
@@ -10571,9 +10539,7 @@
       <c r="H94">
         <v>3</v>
       </c>
-      <c r="I94" s="19" t="s">
-        <v>1432</v>
-      </c>
+      <c r="I94" s="14"/>
       <c r="J94" t="s">
         <v>21</v>
       </c>
@@ -10621,9 +10587,7 @@
       <c r="H95">
         <v>4</v>
       </c>
-      <c r="I95" s="19" t="s">
-        <v>1432</v>
-      </c>
+      <c r="I95" s="14"/>
       <c r="J95" t="s">
         <v>21</v>
       </c>
@@ -10674,9 +10638,7 @@
       <c r="H96">
         <v>4</v>
       </c>
-      <c r="I96" s="19" t="s">
-        <v>1432</v>
-      </c>
+      <c r="I96" s="14"/>
       <c r="J96" t="s">
         <v>21</v>
       </c>
@@ -10727,9 +10689,7 @@
       <c r="H97">
         <v>4</v>
       </c>
-      <c r="I97" s="19" t="s">
-        <v>1432</v>
-      </c>
+      <c r="I97" s="14"/>
       <c r="J97" t="s">
         <v>21</v>
       </c>
@@ -10772,1062 +10732,1134 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B357E3A0-CAC3-4594-9484-B64331912218}">
-  <dimension ref="A1:W33"/>
+  <dimension ref="A1:X33"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="4" ySplit="1" topLeftCell="E2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="J29" sqref="J29"/>
+      <selection pane="bottomRight" activeCell="E19" sqref="E19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
-    <col min="2" max="2" width="13.54296875" customWidth="1"/>
-    <col min="3" max="3" width="28.1796875" customWidth="1"/>
-    <col min="4" max="4" width="30.36328125" customWidth="1"/>
-    <col min="5" max="5" width="15.36328125" customWidth="1"/>
-    <col min="6" max="6" width="16.6328125" customWidth="1"/>
-    <col min="7" max="7" width="17.453125" customWidth="1"/>
-    <col min="9" max="9" width="36.54296875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="42.81640625" customWidth="1"/>
+    <col min="1" max="1" width="8.7265625" style="16"/>
+    <col min="2" max="2" width="13.54296875" style="16" customWidth="1"/>
+    <col min="3" max="3" width="28.1796875" style="16" customWidth="1"/>
+    <col min="4" max="5" width="30.36328125" style="16" customWidth="1"/>
+    <col min="6" max="6" width="15.36328125" style="16" customWidth="1"/>
+    <col min="7" max="7" width="16.6328125" style="16" customWidth="1"/>
+    <col min="8" max="8" width="17.453125" style="16" customWidth="1"/>
+    <col min="9" max="9" width="8.7265625" style="16"/>
+    <col min="10" max="10" width="36.54296875" style="16" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="42.81640625" style="16" customWidth="1"/>
+    <col min="12" max="16384" width="8.7265625" style="16"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10">
-      <c r="A1" t="s">
+    <row r="1" spans="1:11">
+      <c r="A1" s="16" t="s">
         <v>1425</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="16" t="s">
         <v>79</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="16" t="s">
         <v>80</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="16" t="s">
         <v>81</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" s="16" t="s">
+        <v>1446</v>
+      </c>
+      <c r="F1" s="16" t="s">
         <v>1375</v>
       </c>
-      <c r="F1" s="8" t="s">
+      <c r="G1" s="8" t="s">
         <v>82</v>
       </c>
-      <c r="G1" s="8" t="s">
+      <c r="H1" s="8" t="s">
         <v>83</v>
       </c>
-      <c r="H1" s="8" t="s">
+      <c r="I1" s="8" t="s">
         <v>84</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" s="16" t="s">
         <v>16</v>
       </c>
-      <c r="J1" s="12" t="s">
+      <c r="K1" s="12" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="2" spans="1:10">
-      <c r="A2">
+    <row r="2" spans="1:11">
+      <c r="A2" s="16">
         <v>103</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="16" t="s">
         <v>86</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" s="16" t="s">
         <v>87</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D2" s="16" t="s">
         <v>88</v>
       </c>
-      <c r="F2" t="s">
+      <c r="E2" s="16" t="s">
+        <v>1465</v>
+      </c>
+      <c r="G2" s="16" t="s">
         <v>15</v>
       </c>
-      <c r="G2">
+      <c r="H2" s="16">
         <v>0</v>
       </c>
-      <c r="H2" t="s">
+      <c r="I2" s="16" t="s">
         <v>23</v>
       </c>
-      <c r="I2" t="s">
+      <c r="J2" s="16" t="s">
         <v>1413</v>
       </c>
-      <c r="J2" t="s">
+      <c r="K2" s="16" t="s">
         <v>1373</v>
       </c>
     </row>
-    <row r="3" spans="1:10">
-      <c r="A3">
+    <row r="3" spans="1:11">
+      <c r="A3" s="16">
         <v>11</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="16" t="s">
         <v>86</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C3" s="16" t="s">
         <v>89</v>
       </c>
-      <c r="D3" t="s">
+      <c r="D3" s="16" t="s">
         <v>90</v>
       </c>
-      <c r="E3" t="s">
+      <c r="F3" s="16" t="s">
         <v>135</v>
       </c>
-      <c r="F3" t="s">
+      <c r="G3" s="16" t="s">
         <v>23</v>
       </c>
-      <c r="G3">
+      <c r="H3" s="16">
         <v>0</v>
       </c>
-      <c r="H3" t="s">
+      <c r="I3" s="16" t="s">
         <v>23</v>
       </c>
-      <c r="I3" t="s">
+      <c r="J3" s="16" t="s">
         <v>1409</v>
       </c>
-      <c r="J3" s="15" t="s">
+      <c r="K3" s="17" t="s">
         <v>1380</v>
       </c>
     </row>
-    <row r="4" spans="1:10">
-      <c r="A4">
+    <row r="4" spans="1:11">
+      <c r="A4" s="16">
         <v>3</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" s="16" t="s">
         <v>86</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C4" s="16" t="s">
         <v>91</v>
       </c>
-      <c r="D4" t="s">
+      <c r="D4" s="16" t="s">
         <v>92</v>
       </c>
-      <c r="E4" t="s">
+      <c r="E4" s="16" t="s">
+        <v>1464</v>
+      </c>
+      <c r="F4" s="16" t="s">
         <v>135</v>
       </c>
-      <c r="F4" t="s">
+      <c r="G4" s="16" t="s">
         <v>15</v>
       </c>
-      <c r="G4">
+      <c r="H4" s="16">
         <v>0</v>
       </c>
-      <c r="H4" t="s">
+      <c r="I4" s="16" t="s">
         <v>23</v>
       </c>
-      <c r="I4" t="s">
+      <c r="J4" s="16" t="s">
         <v>1414</v>
       </c>
-      <c r="J4" s="17" t="s">
+      <c r="K4" s="17" t="s">
         <v>1376</v>
       </c>
     </row>
-    <row r="5" spans="1:10">
-      <c r="A5">
+    <row r="5" spans="1:11">
+      <c r="A5" s="16">
         <v>5</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B5" s="16" t="s">
         <v>86</v>
       </c>
-      <c r="C5" t="s">
+      <c r="C5" s="16" t="s">
         <v>93</v>
       </c>
-      <c r="D5" t="s">
+      <c r="D5" s="16" t="s">
         <v>94</v>
       </c>
-      <c r="E5" t="s">
+      <c r="E5" s="16" t="s">
+        <v>1463</v>
+      </c>
+      <c r="F5" s="16" t="s">
         <v>135</v>
       </c>
-      <c r="F5" t="s">
+      <c r="G5" s="16" t="s">
         <v>15</v>
       </c>
-      <c r="G5">
+      <c r="H5" s="16">
         <v>0</v>
       </c>
-      <c r="H5" t="s">
+      <c r="I5" s="16" t="s">
         <v>23</v>
       </c>
-      <c r="I5" t="s">
+      <c r="J5" s="16" t="s">
         <v>1416</v>
       </c>
-      <c r="J5" s="15" t="s">
+      <c r="K5" s="17" t="s">
         <v>1381</v>
       </c>
     </row>
-    <row r="6" spans="1:10">
-      <c r="A6">
+    <row r="6" spans="1:11">
+      <c r="A6" s="16">
         <v>9</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B6" s="16" t="s">
         <v>86</v>
       </c>
-      <c r="C6" t="s">
+      <c r="C6" s="16" t="s">
         <v>95</v>
       </c>
-      <c r="D6" t="s">
+      <c r="D6" s="16" t="s">
         <v>96</v>
       </c>
-      <c r="E6" t="s">
+      <c r="E6" s="16" t="s">
+        <v>1459</v>
+      </c>
+      <c r="F6" s="16" t="s">
         <v>135</v>
       </c>
-      <c r="F6" t="s">
+      <c r="G6" s="16" t="s">
         <v>15</v>
       </c>
-      <c r="G6">
+      <c r="H6" s="16">
         <v>0</v>
       </c>
-      <c r="H6" t="s">
+      <c r="I6" s="16" t="s">
         <v>23</v>
       </c>
-      <c r="I6" t="s">
+      <c r="J6" s="16" t="s">
         <v>1412</v>
       </c>
-      <c r="J6" t="s">
+      <c r="K6" s="16" t="s">
         <v>1417</v>
       </c>
     </row>
-    <row r="7" spans="1:10">
-      <c r="A7">
+    <row r="7" spans="1:11">
+      <c r="A7" s="16">
         <v>13</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B7" s="16" t="s">
         <v>86</v>
       </c>
-      <c r="C7" t="s">
+      <c r="C7" s="16" t="s">
         <v>97</v>
       </c>
-      <c r="D7" t="s">
+      <c r="D7" s="16" t="s">
         <v>98</v>
       </c>
-      <c r="E7" t="s">
+      <c r="F7" s="16" t="s">
         <v>135</v>
       </c>
-      <c r="F7" t="s">
+      <c r="G7" s="16" t="s">
         <v>15</v>
       </c>
-      <c r="G7">
+      <c r="H7" s="16">
         <v>0</v>
       </c>
-      <c r="H7" t="s">
+      <c r="I7" s="16" t="s">
         <v>23</v>
       </c>
-      <c r="I7" t="s">
+      <c r="J7" s="16" t="s">
         <v>1415</v>
       </c>
-      <c r="J7" t="s">
+      <c r="K7" s="16" t="s">
         <v>1378</v>
       </c>
     </row>
-    <row r="8" spans="1:10">
-      <c r="A8">
+    <row r="8" spans="1:11">
+      <c r="A8" s="16">
         <v>17</v>
       </c>
-      <c r="B8" t="s">
+      <c r="B8" s="16" t="s">
         <v>86</v>
       </c>
-      <c r="C8" t="s">
+      <c r="C8" s="16" t="s">
         <v>99</v>
       </c>
-      <c r="D8" t="s">
+      <c r="D8" s="16" t="s">
         <v>100</v>
       </c>
-      <c r="E8" t="s">
+      <c r="E8" s="18" t="s">
+        <v>1447</v>
+      </c>
+      <c r="F8" s="16" t="s">
         <v>1403</v>
       </c>
-      <c r="F8" t="s">
+      <c r="G8" s="16" t="s">
         <v>15</v>
       </c>
-      <c r="G8">
+      <c r="H8" s="16">
         <v>0</v>
       </c>
-      <c r="H8" t="s">
+      <c r="I8" s="16" t="s">
         <v>23</v>
       </c>
-      <c r="I8" t="s">
+      <c r="J8" s="16" t="s">
         <v>1407</v>
       </c>
-      <c r="J8" s="15" t="s">
+      <c r="K8" s="17" t="s">
         <v>1400</v>
       </c>
     </row>
-    <row r="9" spans="1:10">
-      <c r="A9">
+    <row r="9" spans="1:11">
+      <c r="A9" s="16">
         <v>23</v>
       </c>
-      <c r="B9" t="s">
+      <c r="B9" s="16" t="s">
         <v>86</v>
       </c>
-      <c r="C9" t="s">
+      <c r="C9" s="16" t="s">
         <v>99</v>
       </c>
-      <c r="D9" t="s">
+      <c r="D9" s="16" t="s">
         <v>101</v>
       </c>
-      <c r="E9" t="s">
+      <c r="E9" s="16" t="s">
+        <v>1469</v>
+      </c>
+      <c r="F9" s="16" t="s">
         <v>1411</v>
       </c>
-      <c r="F9" t="s">
+      <c r="G9" s="16" t="s">
         <v>23</v>
       </c>
-      <c r="G9">
+      <c r="H9" s="16">
         <v>0</v>
       </c>
-      <c r="H9" t="s">
+      <c r="I9" s="16" t="s">
         <v>23</v>
       </c>
-      <c r="I9" t="s">
+      <c r="J9" s="16" t="s">
         <v>1408</v>
       </c>
     </row>
-    <row r="10" spans="1:10">
-      <c r="A10">
+    <row r="10" spans="1:11">
+      <c r="A10" s="16">
         <v>106</v>
       </c>
-      <c r="B10" t="s">
+      <c r="B10" s="16" t="s">
         <v>86</v>
       </c>
-      <c r="C10" t="s">
+      <c r="C10" s="16" t="s">
         <v>102</v>
       </c>
-      <c r="D10" t="s">
+      <c r="D10" s="16" t="s">
         <v>103</v>
       </c>
-      <c r="E10" t="s">
+      <c r="E10" s="16" t="s">
+        <v>1450</v>
+      </c>
+      <c r="F10" s="16" t="s">
         <v>135</v>
       </c>
-      <c r="F10" t="s">
+      <c r="G10" s="16" t="s">
         <v>23</v>
       </c>
-      <c r="G10" t="s">
+      <c r="H10" s="16" t="s">
         <v>23</v>
       </c>
-      <c r="H10" t="s">
+      <c r="I10" s="16" t="s">
         <v>23</v>
       </c>
-      <c r="I10" t="s">
+      <c r="J10" s="16" t="s">
         <v>1410</v>
       </c>
-      <c r="J10" t="s">
+      <c r="K10" s="16" t="s">
         <v>1377</v>
       </c>
     </row>
-    <row r="11" spans="1:10">
-      <c r="A11">
+    <row r="11" spans="1:11">
+      <c r="A11" s="16">
         <v>108</v>
       </c>
-      <c r="B11" t="s">
+      <c r="B11" s="16" t="s">
         <v>86</v>
       </c>
-      <c r="C11" t="s">
+      <c r="C11" s="16" t="s">
         <v>104</v>
       </c>
-      <c r="D11" t="s">
+      <c r="D11" s="16" t="s">
         <v>105</v>
       </c>
-      <c r="E11" t="s">
+      <c r="E11" s="16" t="s">
+        <v>1447</v>
+      </c>
+      <c r="F11" s="16" t="s">
         <v>135</v>
       </c>
-      <c r="F11" t="s">
+      <c r="G11" s="16" t="s">
         <v>15</v>
       </c>
-      <c r="G11">
+      <c r="H11" s="16">
         <v>0</v>
       </c>
-      <c r="H11" t="s">
+      <c r="I11" s="16" t="s">
         <v>23</v>
       </c>
-      <c r="I11" t="s">
+      <c r="J11" s="16" t="s">
         <v>1406</v>
       </c>
-      <c r="J11" s="15" t="s">
+      <c r="K11" s="17" t="s">
         <v>1374</v>
       </c>
     </row>
-    <row r="12" spans="1:10">
-      <c r="A12">
+    <row r="12" spans="1:11">
+      <c r="A12" s="16">
         <v>110</v>
       </c>
-      <c r="B12" t="s">
+      <c r="B12" s="16" t="s">
         <v>106</v>
       </c>
-      <c r="C12" t="s">
+      <c r="C12" s="16" t="s">
         <v>107</v>
       </c>
-      <c r="D12" t="s">
+      <c r="D12" s="16" t="s">
         <v>108</v>
       </c>
-      <c r="E12" t="s">
+      <c r="E12" s="16" t="s">
+        <v>1467</v>
+      </c>
+      <c r="F12" s="16" t="s">
         <v>135</v>
       </c>
-      <c r="F12" t="s">
+      <c r="G12" s="16" t="s">
         <v>15</v>
       </c>
-      <c r="G12">
+      <c r="H12" s="16">
         <v>0</v>
       </c>
-      <c r="H12" t="s">
+      <c r="I12" s="16" t="s">
         <v>23</v>
       </c>
-      <c r="I12" t="s">
+      <c r="J12" s="16" t="s">
         <v>1422</v>
       </c>
-      <c r="J12" s="13" t="s">
+      <c r="K12" s="16" t="s">
         <v>1073</v>
       </c>
     </row>
-    <row r="13" spans="1:10">
-      <c r="A13">
+    <row r="13" spans="1:11">
+      <c r="A13" s="16">
         <v>1</v>
       </c>
-      <c r="B13" t="s">
+      <c r="B13" s="16" t="s">
         <v>106</v>
       </c>
-      <c r="C13" t="s">
+      <c r="C13" s="16" t="s">
         <v>109</v>
       </c>
-      <c r="D13" t="s">
+      <c r="D13" s="16" t="s">
         <v>110</v>
       </c>
-      <c r="E13" t="s">
+      <c r="F13" s="16" t="s">
         <v>135</v>
       </c>
-      <c r="F13" t="s">
+      <c r="G13" s="16" t="s">
         <v>15</v>
       </c>
-      <c r="G13">
+      <c r="H13" s="16">
         <v>0</v>
       </c>
-      <c r="H13" t="s">
+      <c r="I13" s="16" t="s">
         <v>23</v>
       </c>
-      <c r="J13" t="s">
+      <c r="K13" s="16" t="s">
         <v>1379</v>
       </c>
     </row>
-    <row r="14" spans="1:10">
-      <c r="A14">
+    <row r="14" spans="1:11">
+      <c r="A14" s="16">
         <v>8</v>
       </c>
-      <c r="B14" t="s">
+      <c r="B14" s="16" t="s">
         <v>106</v>
       </c>
-      <c r="C14" t="s">
+      <c r="C14" s="16" t="s">
         <v>111</v>
       </c>
-      <c r="D14" t="s">
+      <c r="D14" s="16" t="s">
         <v>112</v>
       </c>
-      <c r="E14" t="s">
+      <c r="E14" s="16" t="s">
+        <v>1459</v>
+      </c>
+      <c r="F14" s="16" t="s">
         <v>135</v>
       </c>
-      <c r="F14" t="s">
+      <c r="G14" s="16" t="s">
         <v>15</v>
       </c>
-      <c r="G14">
+      <c r="H14" s="16">
         <v>2</v>
       </c>
-      <c r="H14" t="s">
+      <c r="I14" s="16" t="s">
         <v>145</v>
       </c>
-      <c r="I14" t="s">
+      <c r="J14" s="16" t="s">
         <v>1383</v>
       </c>
-      <c r="J14" t="s">
+      <c r="K14" s="16" t="s">
         <v>1382</v>
       </c>
     </row>
-    <row r="15" spans="1:10">
-      <c r="A15">
+    <row r="15" spans="1:11">
+      <c r="A15" s="16">
         <v>105</v>
       </c>
-      <c r="B15" t="s">
+      <c r="B15" s="16" t="s">
         <v>106</v>
       </c>
-      <c r="C15" t="s">
+      <c r="C15" s="16" t="s">
         <v>113</v>
       </c>
-      <c r="D15" t="s">
+      <c r="D15" s="16" t="s">
         <v>114</v>
       </c>
-      <c r="E15" t="s">
+      <c r="F15" s="16" t="s">
         <v>135</v>
       </c>
-      <c r="F15" t="s">
+      <c r="G15" s="16" t="s">
         <v>15</v>
       </c>
-      <c r="G15">
+      <c r="H15" s="16">
         <v>0</v>
       </c>
-      <c r="H15" t="s">
+      <c r="I15" s="16" t="s">
         <v>23</v>
       </c>
-      <c r="I15" t="s">
+      <c r="J15" s="16" t="s">
         <v>1385</v>
       </c>
-      <c r="J15" t="s">
+      <c r="K15" s="16" t="s">
         <v>1384</v>
       </c>
     </row>
-    <row r="16" spans="1:10">
-      <c r="A16">
+    <row r="16" spans="1:11">
+      <c r="A16" s="16">
         <v>19</v>
       </c>
-      <c r="B16" t="s">
+      <c r="B16" s="16" t="s">
         <v>106</v>
       </c>
-      <c r="C16" t="s">
+      <c r="C16" s="16" t="s">
         <v>115</v>
       </c>
-      <c r="D16" t="s">
+      <c r="D16" s="16" t="s">
         <v>116</v>
       </c>
-      <c r="E16" t="s">
+      <c r="F16" s="16" t="s">
         <v>135</v>
       </c>
-      <c r="F16" t="s">
+      <c r="G16" s="16" t="s">
         <v>15</v>
       </c>
-      <c r="G16">
+      <c r="H16" s="16">
         <v>2</v>
       </c>
-      <c r="H16" t="s">
+      <c r="I16" s="16" t="s">
         <v>145</v>
       </c>
-      <c r="I16" t="s">
+      <c r="J16" s="16" t="s">
         <v>1387</v>
       </c>
-      <c r="J16" t="s">
+      <c r="K16" s="16" t="s">
         <v>1388</v>
       </c>
     </row>
-    <row r="17" spans="1:23">
-      <c r="A17">
+    <row r="17" spans="1:24">
+      <c r="A17" s="16">
         <v>25</v>
       </c>
-      <c r="B17" t="s">
+      <c r="B17" s="16" t="s">
         <v>106</v>
       </c>
-      <c r="C17" t="s">
+      <c r="C17" s="16" t="s">
         <v>117</v>
       </c>
-      <c r="D17" t="s">
+      <c r="D17" s="16" t="s">
         <v>118</v>
       </c>
-      <c r="E17" t="s">
+      <c r="E17" s="16" t="s">
+        <v>1466</v>
+      </c>
+      <c r="F17" s="16" t="s">
         <v>135</v>
       </c>
-      <c r="F17" t="s">
+      <c r="G17" s="16" t="s">
         <v>15</v>
       </c>
-      <c r="G17">
+      <c r="H17" s="16">
         <v>1</v>
       </c>
-      <c r="H17" t="s">
+      <c r="I17" s="16" t="s">
         <v>1390</v>
       </c>
-      <c r="I17" t="s">
+      <c r="J17" s="16" t="s">
         <v>1405</v>
       </c>
-      <c r="J17" t="s">
+      <c r="K17" s="16" t="s">
         <v>1389</v>
       </c>
-      <c r="W17" s="18" t="s">
+      <c r="X17" s="19" t="s">
         <v>1404</v>
       </c>
     </row>
-    <row r="18" spans="1:23">
-      <c r="A18">
+    <row r="18" spans="1:24">
+      <c r="A18" s="16">
         <v>26</v>
       </c>
-      <c r="B18" t="s">
+      <c r="B18" s="16" t="s">
         <v>106</v>
       </c>
-      <c r="C18" t="s">
+      <c r="C18" s="16" t="s">
         <v>119</v>
       </c>
-      <c r="D18" t="s">
+      <c r="D18" s="16" t="s">
         <v>120</v>
       </c>
-      <c r="E18" t="s">
+      <c r="F18" s="16" t="s">
         <v>135</v>
       </c>
-      <c r="F18" t="s">
+      <c r="G18" s="16" t="s">
         <v>15</v>
       </c>
-      <c r="G18">
+      <c r="H18" s="16">
         <v>0</v>
       </c>
-      <c r="H18" t="s">
+      <c r="I18" s="16" t="s">
         <v>23</v>
       </c>
-      <c r="J18" t="s">
+      <c r="K18" s="16" t="s">
         <v>1391</v>
       </c>
     </row>
-    <row r="19" spans="1:23">
-      <c r="A19">
+    <row r="19" spans="1:24">
+      <c r="A19" s="16">
         <v>7</v>
       </c>
-      <c r="B19" t="s">
+      <c r="B19" s="16" t="s">
         <v>106</v>
       </c>
-      <c r="C19" t="s">
+      <c r="C19" s="16" t="s">
         <v>121</v>
       </c>
-      <c r="D19" t="s">
+      <c r="D19" s="16" t="s">
         <v>122</v>
       </c>
-      <c r="E19" t="s">
+      <c r="F19" s="16" t="s">
         <v>135</v>
       </c>
-      <c r="F19" t="s">
+      <c r="G19" s="16" t="s">
         <v>15</v>
       </c>
-      <c r="G19">
+      <c r="H19" s="16">
         <v>1</v>
       </c>
-      <c r="H19" t="s">
+      <c r="I19" s="16" t="s">
         <v>145</v>
       </c>
-      <c r="I19" t="s">
+      <c r="J19" s="16" t="s">
         <v>1392</v>
       </c>
-      <c r="J19" t="s">
+      <c r="K19" s="16" t="s">
         <v>618</v>
       </c>
     </row>
-    <row r="20" spans="1:23">
-      <c r="A20">
+    <row r="20" spans="1:24">
+      <c r="A20" s="16">
         <v>14</v>
       </c>
-      <c r="B20" t="s">
+      <c r="B20" s="16" t="s">
         <v>106</v>
       </c>
-      <c r="C20" t="s">
+      <c r="C20" s="16" t="s">
         <v>123</v>
       </c>
-      <c r="D20" t="s">
+      <c r="D20" s="16" t="s">
         <v>124</v>
       </c>
-      <c r="E20" s="19" t="s">
+      <c r="E20" s="16" t="s">
+        <v>1462</v>
+      </c>
+      <c r="F20" s="18" t="s">
         <v>15</v>
       </c>
-      <c r="F20" t="s">
+      <c r="G20" s="16" t="s">
         <v>15</v>
       </c>
-      <c r="G20">
+      <c r="H20" s="16">
         <v>0</v>
       </c>
-      <c r="H20" t="s">
+      <c r="I20" s="16" t="s">
         <v>23</v>
       </c>
-      <c r="I20" t="s">
+      <c r="J20" s="16" t="s">
         <v>1423</v>
       </c>
-      <c r="J20" t="s">
+      <c r="K20" s="16" t="s">
         <v>1395</v>
       </c>
     </row>
-    <row r="21" spans="1:23" ht="15" customHeight="1">
-      <c r="A21">
+    <row r="21" spans="1:24" ht="15" customHeight="1">
+      <c r="A21" s="16">
         <v>22</v>
       </c>
-      <c r="B21" t="s">
+      <c r="B21" s="16" t="s">
         <v>106</v>
       </c>
-      <c r="C21" t="s">
+      <c r="C21" s="16" t="s">
         <v>125</v>
       </c>
-      <c r="D21" s="13" t="s">
+      <c r="D21" s="16" t="s">
         <v>126</v>
       </c>
-      <c r="E21" s="13" t="s">
+      <c r="F21" s="16" t="s">
         <v>135</v>
       </c>
-      <c r="F21" t="s">
+      <c r="G21" s="16" t="s">
         <v>15</v>
       </c>
-      <c r="G21">
+      <c r="H21" s="16">
         <v>0</v>
       </c>
-      <c r="H21" t="s">
+      <c r="I21" s="16" t="s">
         <v>23</v>
       </c>
-      <c r="I21" t="s">
+      <c r="J21" s="16" t="s">
         <v>1399</v>
       </c>
-      <c r="J21" t="s">
+      <c r="K21" s="16" t="s">
         <v>1397</v>
       </c>
     </row>
-    <row r="22" spans="1:23">
-      <c r="A22">
+    <row r="22" spans="1:24">
+      <c r="A22" s="16">
         <v>24</v>
       </c>
-      <c r="B22" t="s">
+      <c r="B22" s="16" t="s">
         <v>127</v>
       </c>
-      <c r="C22" t="s">
+      <c r="C22" s="16" t="s">
         <v>128</v>
       </c>
-      <c r="D22" t="s">
+      <c r="D22" s="16" t="s">
         <v>129</v>
       </c>
-      <c r="E22" t="s">
+      <c r="F22" s="16" t="s">
         <v>135</v>
       </c>
-      <c r="F22" t="s">
+      <c r="G22" s="16" t="s">
         <v>15</v>
       </c>
-      <c r="G22">
+      <c r="H22" s="16">
         <v>0</v>
       </c>
-      <c r="H22" t="s">
+      <c r="I22" s="16" t="s">
         <v>23</v>
       </c>
-      <c r="J22" t="s">
+      <c r="K22" s="16" t="s">
         <v>1398</v>
       </c>
     </row>
-    <row r="23" spans="1:23" ht="15.5">
-      <c r="A23">
+    <row r="23" spans="1:24" ht="15.5">
+      <c r="A23" s="16">
         <v>27</v>
       </c>
-      <c r="B23" t="s">
+      <c r="B23" s="16" t="s">
         <v>127</v>
       </c>
-      <c r="C23" t="s">
+      <c r="C23" s="16" t="s">
         <v>130</v>
       </c>
-      <c r="D23" t="s">
+      <c r="D23" s="16" t="s">
         <v>131</v>
       </c>
-      <c r="E23" t="s">
+      <c r="F23" s="16" t="s">
         <v>135</v>
       </c>
-      <c r="F23" t="s">
+      <c r="G23" s="16" t="s">
         <v>15</v>
       </c>
-      <c r="G23">
+      <c r="H23" s="16">
         <v>0</v>
       </c>
-      <c r="H23" t="s">
+      <c r="I23" s="16" t="s">
         <v>23</v>
       </c>
-      <c r="J23" s="14" t="s">
+      <c r="K23" s="20" t="s">
         <v>132</v>
       </c>
     </row>
-    <row r="24" spans="1:23">
-      <c r="A24">
+    <row r="24" spans="1:24">
+      <c r="A24" s="16">
         <v>28</v>
       </c>
-      <c r="B24" t="s">
+      <c r="B24" s="16" t="s">
         <v>127</v>
       </c>
-      <c r="C24" t="s">
+      <c r="C24" s="16" t="s">
         <v>133</v>
       </c>
-      <c r="D24" t="s">
+      <c r="D24" s="16" t="s">
         <v>134</v>
       </c>
-      <c r="E24" t="s">
+      <c r="E24" s="16" t="s">
+        <v>1468</v>
+      </c>
+      <c r="F24" s="16" t="s">
         <v>135</v>
       </c>
-      <c r="F24" t="s">
+      <c r="G24" s="16" t="s">
         <v>15</v>
       </c>
-      <c r="G24">
+      <c r="H24" s="16">
         <v>0</v>
       </c>
-      <c r="H24" t="s">
+      <c r="I24" s="16" t="s">
         <v>23</v>
       </c>
-      <c r="I24" t="s">
+      <c r="J24" s="16" t="s">
         <v>1386</v>
       </c>
-      <c r="J24" s="15" t="s">
+      <c r="K24" s="17" t="s">
         <v>137</v>
       </c>
     </row>
-    <row r="25" spans="1:23">
-      <c r="A25">
+    <row r="25" spans="1:24">
+      <c r="A25" s="16">
         <v>28</v>
       </c>
-      <c r="B25" t="s">
+      <c r="B25" s="16" t="s">
         <v>127</v>
       </c>
-      <c r="C25" t="s">
+      <c r="C25" s="16" t="s">
         <v>138</v>
       </c>
-      <c r="D25" t="s">
+      <c r="D25" s="16" t="s">
         <v>134</v>
       </c>
-      <c r="E25" t="s">
+      <c r="E25" s="16" t="s">
+        <v>1468</v>
+      </c>
+      <c r="F25" s="16" t="s">
         <v>135</v>
       </c>
-      <c r="F25" t="s">
+      <c r="G25" s="16" t="s">
         <v>15</v>
       </c>
-      <c r="G25">
+      <c r="H25" s="16">
         <v>0</v>
       </c>
-      <c r="H25" t="s">
+      <c r="I25" s="16" t="s">
         <v>23</v>
       </c>
-      <c r="I25" t="s">
+      <c r="J25" s="16" t="s">
         <v>1386</v>
       </c>
-      <c r="J25" s="15" t="s">
+      <c r="K25" s="17" t="s">
         <v>137</v>
       </c>
     </row>
-    <row r="26" spans="1:23" ht="29">
-      <c r="A26">
+    <row r="26" spans="1:24" ht="15.5">
+      <c r="A26" s="16">
         <v>102</v>
       </c>
-      <c r="B26" t="s">
+      <c r="B26" s="16" t="s">
         <v>127</v>
       </c>
-      <c r="C26" t="s">
+      <c r="C26" s="16" t="s">
         <v>139</v>
       </c>
-      <c r="D26" t="s">
+      <c r="D26" s="16" t="s">
         <v>140</v>
       </c>
-      <c r="E26" t="s">
+      <c r="E26" s="16" t="s">
+        <v>1461</v>
+      </c>
+      <c r="F26" s="16" t="s">
         <v>135</v>
       </c>
-      <c r="F26" t="s">
+      <c r="G26" s="16" t="s">
         <v>15</v>
       </c>
-      <c r="G26">
+      <c r="H26" s="16">
         <v>0</v>
       </c>
-      <c r="H26" t="s">
+      <c r="I26" s="16" t="s">
         <v>23</v>
       </c>
-      <c r="I26" s="13" t="s">
+      <c r="J26" s="16" t="s">
         <v>142</v>
       </c>
-      <c r="J26" s="16" t="s">
+      <c r="K26" s="21" t="s">
         <v>141</v>
       </c>
     </row>
-    <row r="27" spans="1:23" ht="29">
-      <c r="A27">
+    <row r="27" spans="1:24" ht="15.5">
+      <c r="A27" s="16">
         <v>111</v>
       </c>
-      <c r="B27" t="s">
+      <c r="B27" s="16" t="s">
         <v>127</v>
       </c>
-      <c r="C27" t="s">
+      <c r="C27" s="16" t="s">
         <v>143</v>
       </c>
-      <c r="D27" t="s">
+      <c r="D27" s="16" t="s">
         <v>144</v>
       </c>
-      <c r="E27" t="s">
+      <c r="E27" s="16" t="s">
+        <v>1447</v>
+      </c>
+      <c r="F27" s="16" t="s">
         <v>135</v>
       </c>
-      <c r="F27" t="s">
+      <c r="G27" s="16" t="s">
         <v>135</v>
       </c>
-      <c r="G27">
+      <c r="H27" s="16">
         <v>1</v>
       </c>
-      <c r="H27" t="s">
+      <c r="I27" s="16" t="s">
         <v>145</v>
       </c>
-      <c r="I27" s="13" t="s">
+      <c r="J27" s="16" t="s">
         <v>147</v>
       </c>
-      <c r="J27" s="16" t="s">
+      <c r="K27" s="21" t="s">
         <v>146</v>
       </c>
     </row>
-    <row r="28" spans="1:23" ht="15.5">
-      <c r="A28">
+    <row r="28" spans="1:24" ht="15.5">
+      <c r="A28" s="16">
         <v>112</v>
       </c>
-      <c r="B28" t="s">
+      <c r="B28" s="16" t="s">
         <v>127</v>
       </c>
-      <c r="C28" t="s">
+      <c r="C28" s="16" t="s">
         <v>148</v>
       </c>
-      <c r="D28" t="s">
+      <c r="D28" s="16" t="s">
         <v>96</v>
       </c>
-      <c r="E28" t="s">
+      <c r="E28" s="16" t="s">
+        <v>1459</v>
+      </c>
+      <c r="F28" s="16" t="s">
         <v>135</v>
       </c>
-      <c r="F28" t="s">
+      <c r="G28" s="16" t="s">
         <v>1421</v>
       </c>
-      <c r="G28">
+      <c r="H28" s="16">
         <v>1</v>
       </c>
-      <c r="H28" t="s">
+      <c r="I28" s="16" t="s">
         <v>136</v>
       </c>
-      <c r="J28" s="16" t="s">
+      <c r="K28" s="21" t="s">
         <v>149</v>
       </c>
     </row>
-    <row r="29" spans="1:23">
-      <c r="A29">
+    <row r="29" spans="1:24">
+      <c r="A29" s="16">
         <v>113</v>
       </c>
-      <c r="B29" t="s">
+      <c r="B29" s="16" t="s">
         <v>127</v>
       </c>
-      <c r="C29" t="s">
+      <c r="C29" s="16" t="s">
         <v>150</v>
       </c>
-      <c r="D29" t="s">
+      <c r="D29" s="16" t="s">
         <v>151</v>
       </c>
-      <c r="E29" t="s">
+      <c r="E29" s="16" t="s">
+        <v>1459</v>
+      </c>
+      <c r="F29" s="16" t="s">
         <v>135</v>
       </c>
-      <c r="F29" t="s">
+      <c r="G29" s="16" t="s">
         <v>135</v>
       </c>
-      <c r="G29">
+      <c r="H29" s="16">
         <v>1</v>
       </c>
-      <c r="H29" t="s">
+      <c r="I29" s="16" t="s">
         <v>145</v>
       </c>
-      <c r="J29" t="s">
+      <c r="K29" s="16" t="s">
         <v>1396</v>
       </c>
     </row>
-    <row r="30" spans="1:23">
-      <c r="A30">
+    <row r="30" spans="1:24">
+      <c r="A30" s="16">
         <v>113</v>
       </c>
-      <c r="B30" t="s">
+      <c r="B30" s="16" t="s">
         <v>127</v>
       </c>
-      <c r="C30" t="s">
+      <c r="C30" s="16" t="s">
         <v>150</v>
       </c>
-      <c r="D30" t="s">
+      <c r="D30" s="16" t="s">
         <v>151</v>
       </c>
-      <c r="E30" t="s">
+      <c r="E30" s="16" t="s">
+        <v>1459</v>
+      </c>
+      <c r="F30" s="16" t="s">
         <v>1418</v>
       </c>
-      <c r="F30" t="s">
+      <c r="G30" s="16" t="s">
         <v>135</v>
       </c>
-      <c r="G30">
+      <c r="H30" s="16">
         <v>4</v>
       </c>
-      <c r="H30" t="s">
+      <c r="I30" s="16" t="s">
         <v>145</v>
       </c>
-      <c r="J30" t="s">
+      <c r="K30" s="16" t="s">
         <v>1396</v>
       </c>
     </row>
-    <row r="31" spans="1:23" ht="15.5">
-      <c r="A31">
+    <row r="31" spans="1:24" ht="15.5">
+      <c r="A31" s="16">
         <v>104</v>
       </c>
-      <c r="B31" t="s">
+      <c r="B31" s="16" t="s">
         <v>127</v>
       </c>
-      <c r="C31" t="s">
+      <c r="C31" s="16" t="s">
         <v>152</v>
       </c>
-      <c r="D31" t="s">
+      <c r="D31" s="16" t="s">
         <v>103</v>
       </c>
-      <c r="E31" t="s">
+      <c r="E31" s="16" t="s">
+        <v>1460</v>
+      </c>
+      <c r="F31" s="16" t="s">
         <v>135</v>
       </c>
-      <c r="F31" t="s">
+      <c r="G31" s="16" t="s">
         <v>15</v>
       </c>
-      <c r="G31">
+      <c r="H31" s="16">
         <v>0</v>
       </c>
-      <c r="H31" t="s">
+      <c r="I31" s="16" t="s">
         <v>23</v>
       </c>
-      <c r="J31" s="16" t="s">
+      <c r="K31" s="21" t="s">
         <v>153</v>
       </c>
     </row>
-    <row r="32" spans="1:23" ht="15.5">
-      <c r="A32">
+    <row r="32" spans="1:24" ht="15.5">
+      <c r="A32" s="16">
         <v>107</v>
       </c>
-      <c r="B32" t="s">
+      <c r="B32" s="16" t="s">
         <v>127</v>
       </c>
-      <c r="C32" t="s">
+      <c r="C32" s="16" t="s">
         <v>154</v>
       </c>
-      <c r="D32" t="s">
+      <c r="D32" s="16" t="s">
         <v>155</v>
       </c>
-      <c r="E32" t="s">
+      <c r="E32" s="16" t="s">
+        <v>1447</v>
+      </c>
+      <c r="F32" s="16" t="s">
         <v>135</v>
       </c>
-      <c r="F32" t="s">
+      <c r="G32" s="16" t="s">
         <v>15</v>
       </c>
-      <c r="G32">
+      <c r="H32" s="16">
         <v>0</v>
       </c>
-      <c r="H32" t="s">
+      <c r="I32" s="16" t="s">
         <v>23</v>
       </c>
-      <c r="J32" s="16" t="s">
+      <c r="K32" s="21" t="s">
         <v>156</v>
       </c>
     </row>
-    <row r="33" spans="1:10" ht="15.5">
-      <c r="A33">
+    <row r="33" spans="1:11" ht="15.5">
+      <c r="A33" s="16">
         <v>101</v>
       </c>
-      <c r="B33" t="s">
+      <c r="B33" s="16" t="s">
         <v>127</v>
       </c>
-      <c r="C33" t="s">
+      <c r="C33" s="16" t="s">
         <v>157</v>
       </c>
-      <c r="D33" t="s">
+      <c r="D33" s="16" t="s">
         <v>158</v>
       </c>
-      <c r="E33" t="s">
+      <c r="E33" s="16" t="s">
+        <v>1460</v>
+      </c>
+      <c r="F33" s="16" t="s">
         <v>135</v>
       </c>
-      <c r="F33" t="s">
+      <c r="G33" s="16" t="s">
         <v>15</v>
       </c>
-      <c r="G33">
+      <c r="H33" s="16">
         <v>0</v>
       </c>
-      <c r="H33" t="s">
+      <c r="I33" s="16" t="s">
         <v>23</v>
       </c>
-      <c r="I33" s="13" t="s">
+      <c r="J33" s="16" t="s">
         <v>1394</v>
       </c>
-      <c r="J33" s="16" t="s">
+      <c r="K33" s="21" t="s">
         <v>1393</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="J24" r:id="rId1" xr:uid="{8074BD4A-B3AC-47CB-B325-D7D9351C49E5}"/>
-    <hyperlink ref="J25" r:id="rId2" xr:uid="{8D031A30-0D37-4B44-872D-F806A41DB8C5}"/>
-    <hyperlink ref="J11" r:id="rId3" xr:uid="{1E37F82F-F8B1-4735-A08D-AF932314E934}"/>
-    <hyperlink ref="J4" r:id="rId4" xr:uid="{233F6465-2675-43E3-92B4-611CB5D21380}"/>
-    <hyperlink ref="J3" r:id="rId5" xr:uid="{9B3DD1E3-DA00-46FB-9DDF-B907B11135A9}"/>
-    <hyperlink ref="J5" r:id="rId6" xr:uid="{E20C66EA-3F4D-4F55-A35B-00A128CF9356}"/>
-    <hyperlink ref="J8" r:id="rId7" xr:uid="{00149E17-6012-476F-9B85-96D5DBDC70A9}"/>
+    <hyperlink ref="K24" r:id="rId1" xr:uid="{8074BD4A-B3AC-47CB-B325-D7D9351C49E5}"/>
+    <hyperlink ref="K25" r:id="rId2" xr:uid="{8D031A30-0D37-4B44-872D-F806A41DB8C5}"/>
+    <hyperlink ref="K11" r:id="rId3" xr:uid="{1E37F82F-F8B1-4735-A08D-AF932314E934}"/>
+    <hyperlink ref="K4" r:id="rId4" xr:uid="{233F6465-2675-43E3-92B4-611CB5D21380}"/>
+    <hyperlink ref="K3" r:id="rId5" xr:uid="{9B3DD1E3-DA00-46FB-9DDF-B907B11135A9}"/>
+    <hyperlink ref="K5" r:id="rId6" xr:uid="{E20C66EA-3F4D-4F55-A35B-00A128CF9356}"/>
+    <hyperlink ref="K8" r:id="rId7" xr:uid="{00149E17-6012-476F-9B85-96D5DBDC70A9}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -12007,11 +12039,11 @@
       <c r="AE3" s="3"/>
     </row>
     <row r="4" spans="1:31">
-      <c r="A4" s="20" t="s">
+      <c r="A4" s="15" t="s">
         <v>181</v>
       </c>
-      <c r="B4" s="20"/>
-      <c r="C4" s="20"/>
+      <c r="B4" s="15"/>
+      <c r="C4" s="15"/>
       <c r="D4" s="5">
         <v>33284114</v>
       </c>
@@ -12501,11 +12533,11 @@
       <c r="AE13" s="3"/>
     </row>
     <row r="14" spans="1:31">
-      <c r="A14" s="20" t="s">
+      <c r="A14" s="15" t="s">
         <v>181</v>
       </c>
-      <c r="B14" s="20"/>
-      <c r="C14" s="20"/>
+      <c r="B14" s="15"/>
+      <c r="C14" s="15"/>
       <c r="D14" s="5">
         <v>33230550</v>
       </c>
@@ -12942,11 +12974,11 @@
       <c r="AE22" s="3"/>
     </row>
     <row r="23" spans="1:31">
-      <c r="A23" s="20" t="s">
+      <c r="A23" s="15" t="s">
         <v>256</v>
       </c>
-      <c r="B23" s="20"/>
-      <c r="C23" s="20"/>
+      <c r="B23" s="15"/>
+      <c r="C23" s="15"/>
       <c r="D23" s="5">
         <v>35344464</v>
       </c>
@@ -13115,19 +13147,19 @@
       <c r="L26" s="2"/>
       <c r="M26" s="2"/>
       <c r="N26" s="2"/>
-      <c r="O26" s="20"/>
-      <c r="P26" s="20"/>
+      <c r="O26" s="15"/>
+      <c r="P26" s="15"/>
       <c r="Q26" s="2"/>
       <c r="R26" s="2"/>
       <c r="S26" s="2"/>
       <c r="T26" s="2"/>
-      <c r="U26" s="20"/>
-      <c r="V26" s="20"/>
+      <c r="U26" s="15"/>
+      <c r="V26" s="15"/>
       <c r="W26" s="2"/>
       <c r="X26" s="2"/>
       <c r="Y26" s="2"/>
-      <c r="Z26" s="20"/>
-      <c r="AA26" s="20"/>
+      <c r="Z26" s="15"/>
+      <c r="AA26" s="15"/>
       <c r="AB26" s="2"/>
       <c r="AC26" s="2"/>
       <c r="AD26" s="2"/>
@@ -13569,8 +13601,8 @@
       <c r="S35" s="3"/>
       <c r="T35" s="3"/>
       <c r="U35" s="2"/>
-      <c r="V35" s="20"/>
-      <c r="W35" s="20"/>
+      <c r="V35" s="15"/>
+      <c r="W35" s="15"/>
       <c r="X35" s="3"/>
       <c r="Y35" s="3"/>
       <c r="Z35" s="3"/>

</xml_diff>

<commit_message>
formatted a data entry
</commit_message>
<xml_diff>
--- a/hexa_review.xlsx
+++ b/hexa_review.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://bmgf-my.sharepoint.com/personal/qifang_bi_gatesfoundation_org/Documents/Repository/hexa_dosing/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="2112" documentId="8_{3E1959A5-03D9-489A-814E-73E2A90AC25F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{71CBB789-CB68-460F-A8A1-B9FF66E8ACF9}"/>
+  <xr:revisionPtr revIDLastSave="2114" documentId="8_{3E1959A5-03D9-489A-814E-73E2A90AC25F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{9EE2C389-BD91-49C7-A01E-727813F0A98F}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11620" activeTab="2" xr2:uid="{6686FE0B-19D2-4DD2-8D2B-E91F6EF7CA1A}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11620" activeTab="1" xr2:uid="{6686FE0B-19D2-4DD2-8D2B-E91F6EF7CA1A}"/>
   </bookViews>
   <sheets>
     <sheet name="readme" sheetId="5" r:id="rId1"/>
@@ -4302,9 +4302,6 @@
     <t>https://doi.org/10.1093/infdis/jiw433</t>
   </si>
   <si>
-    <t>Guoyang Liao</t>
-  </si>
-  <si>
     <t>2, 3, 4, 18 months</t>
   </si>
   <si>
@@ -4510,6 +4507,9 @@
   </si>
   <si>
     <t>unspecified "Serum samples were collected fromall infants before and 30 days after vaccination with 3 doses of each vaccine for detection of anti–poliovirus-neutralizing antibodies."</t>
+  </si>
+  <si>
+    <t>Liao G</t>
   </si>
 </sst>
 </file>
@@ -5060,7 +5060,7 @@
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -5096,13 +5096,11 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="26" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="42" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="42" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="43">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -5492,42 +5490,42 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" t="s">
+        <v>1435</v>
+      </c>
+      <c r="B1" t="s">
         <v>1436</v>
-      </c>
-      <c r="B1" t="s">
-        <v>1437</v>
       </c>
     </row>
     <row r="2" spans="1:2">
       <c r="A2" t="s">
+        <v>1437</v>
+      </c>
+      <c r="B2" t="s">
         <v>1438</v>
-      </c>
-      <c r="B2" t="s">
-        <v>1439</v>
       </c>
     </row>
     <row r="3" spans="1:2">
       <c r="A3" t="s">
+        <v>1439</v>
+      </c>
+      <c r="B3" t="s">
         <v>1440</v>
-      </c>
-      <c r="B3" t="s">
-        <v>1441</v>
       </c>
     </row>
     <row r="4" spans="1:2">
       <c r="A4" t="s">
+        <v>1441</v>
+      </c>
+      <c r="B4" t="s">
         <v>1442</v>
-      </c>
-      <c r="B4" t="s">
-        <v>1443</v>
       </c>
     </row>
     <row r="5" spans="1:2">
       <c r="A5" t="s">
-        <v>1445</v>
+        <v>1444</v>
       </c>
       <c r="B5" t="s">
-        <v>1444</v>
+        <v>1443</v>
       </c>
     </row>
   </sheetData>
@@ -5539,8 +5537,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BCECA026-A481-4661-B5E1-656ABE78B0F5}">
   <dimension ref="A1:W1048575"/>
   <sheetViews>
-    <sheetView topLeftCell="A8" zoomScale="91" workbookViewId="0">
-      <selection activeCell="I21" sqref="I21"/>
+    <sheetView tabSelected="1" topLeftCell="A68" zoomScale="91" workbookViewId="0">
+      <selection activeCell="G79" sqref="G79"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -5557,7 +5555,7 @@
   <sheetData>
     <row r="1" spans="1:23">
       <c r="A1" t="s">
-        <v>1425</v>
+        <v>1424</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
@@ -5581,7 +5579,7 @@
         <v>6</v>
       </c>
       <c r="I1" t="s">
-        <v>1446</v>
+        <v>1445</v>
       </c>
       <c r="J1" t="s">
         <v>7</v>
@@ -5779,7 +5777,7 @@
         <v>25</v>
       </c>
       <c r="E5" t="s">
-        <v>1424</v>
+        <v>1423</v>
       </c>
       <c r="F5">
         <v>2022</v>
@@ -5791,7 +5789,7 @@
         <v>3</v>
       </c>
       <c r="I5" t="s">
-        <v>1447</v>
+        <v>1446</v>
       </c>
       <c r="J5" t="s">
         <v>21</v>
@@ -5835,7 +5833,7 @@
         <v>25</v>
       </c>
       <c r="E6" t="s">
-        <v>1424</v>
+        <v>1423</v>
       </c>
       <c r="F6">
         <v>2022</v>
@@ -5847,7 +5845,7 @@
         <v>3</v>
       </c>
       <c r="I6" t="s">
-        <v>1447</v>
+        <v>1446</v>
       </c>
       <c r="J6" t="s">
         <v>21</v>
@@ -5891,7 +5889,7 @@
         <v>25</v>
       </c>
       <c r="E7" t="s">
-        <v>1424</v>
+        <v>1423</v>
       </c>
       <c r="F7">
         <v>2022</v>
@@ -5903,7 +5901,7 @@
         <v>3</v>
       </c>
       <c r="I7" t="s">
-        <v>1447</v>
+        <v>1446</v>
       </c>
       <c r="J7" t="s">
         <v>21</v>
@@ -5947,7 +5945,7 @@
         <v>25</v>
       </c>
       <c r="E8" t="s">
-        <v>1424</v>
+        <v>1423</v>
       </c>
       <c r="F8">
         <v>2022</v>
@@ -6003,7 +6001,7 @@
         <v>25</v>
       </c>
       <c r="E9" t="s">
-        <v>1424</v>
+        <v>1423</v>
       </c>
       <c r="F9">
         <v>2022</v>
@@ -6059,7 +6057,7 @@
         <v>25</v>
       </c>
       <c r="E10" t="s">
-        <v>1424</v>
+        <v>1423</v>
       </c>
       <c r="F10">
         <v>2022</v>
@@ -6115,7 +6113,7 @@
         <v>25</v>
       </c>
       <c r="E11" t="s">
-        <v>1424</v>
+        <v>1423</v>
       </c>
       <c r="F11">
         <v>2022</v>
@@ -6127,7 +6125,7 @@
         <v>3</v>
       </c>
       <c r="I11" t="s">
-        <v>1447</v>
+        <v>1446</v>
       </c>
       <c r="J11" t="s">
         <v>29</v>
@@ -6171,7 +6169,7 @@
         <v>25</v>
       </c>
       <c r="E12" t="s">
-        <v>1424</v>
+        <v>1423</v>
       </c>
       <c r="F12">
         <v>2022</v>
@@ -6183,7 +6181,7 @@
         <v>3</v>
       </c>
       <c r="I12" t="s">
-        <v>1447</v>
+        <v>1446</v>
       </c>
       <c r="J12" t="s">
         <v>29</v>
@@ -6227,7 +6225,7 @@
         <v>25</v>
       </c>
       <c r="E13" t="s">
-        <v>1424</v>
+        <v>1423</v>
       </c>
       <c r="F13">
         <v>2022</v>
@@ -6239,7 +6237,7 @@
         <v>3</v>
       </c>
       <c r="I13" t="s">
-        <v>1447</v>
+        <v>1446</v>
       </c>
       <c r="J13" t="s">
         <v>29</v>
@@ -6283,7 +6281,7 @@
         <v>25</v>
       </c>
       <c r="E14" t="s">
-        <v>1424</v>
+        <v>1423</v>
       </c>
       <c r="F14">
         <v>2022</v>
@@ -6339,7 +6337,7 @@
         <v>25</v>
       </c>
       <c r="E15" t="s">
-        <v>1424</v>
+        <v>1423</v>
       </c>
       <c r="F15">
         <v>2022</v>
@@ -6395,7 +6393,7 @@
         <v>25</v>
       </c>
       <c r="E16" t="s">
-        <v>1424</v>
+        <v>1423</v>
       </c>
       <c r="F16">
         <v>2022</v>
@@ -6463,7 +6461,7 @@
         <v>2</v>
       </c>
       <c r="I17" t="s">
-        <v>1449</v>
+        <v>1448</v>
       </c>
       <c r="J17" t="s">
         <v>29</v>
@@ -6516,7 +6514,7 @@
         <v>2</v>
       </c>
       <c r="I18" t="s">
-        <v>1451</v>
+        <v>1450</v>
       </c>
       <c r="J18" t="s">
         <v>29</v>
@@ -6569,7 +6567,7 @@
         <v>2</v>
       </c>
       <c r="I19" t="s">
-        <v>1452</v>
+        <v>1451</v>
       </c>
       <c r="J19" t="s">
         <v>29</v>
@@ -6622,7 +6620,7 @@
         <v>2</v>
       </c>
       <c r="I20" t="s">
-        <v>1453</v>
+        <v>1452</v>
       </c>
       <c r="J20" t="s">
         <v>29</v>
@@ -6675,7 +6673,7 @@
         <v>2</v>
       </c>
       <c r="I21" t="s">
-        <v>1454</v>
+        <v>1453</v>
       </c>
       <c r="J21" t="s">
         <v>29</v>
@@ -6728,7 +6726,7 @@
         <v>2</v>
       </c>
       <c r="I22" t="s">
-        <v>1455</v>
+        <v>1454</v>
       </c>
       <c r="J22" t="s">
         <v>29</v>
@@ -6781,7 +6779,7 @@
         <v>2</v>
       </c>
       <c r="I23" t="s">
-        <v>1456</v>
+        <v>1455</v>
       </c>
       <c r="J23" t="s">
         <v>29</v>
@@ -6834,7 +6832,7 @@
         <v>2</v>
       </c>
       <c r="I24" t="s">
-        <v>1457</v>
+        <v>1456</v>
       </c>
       <c r="J24" t="s">
         <v>29</v>
@@ -6887,7 +6885,7 @@
         <v>2</v>
       </c>
       <c r="I25" t="s">
-        <v>1458</v>
+        <v>1457</v>
       </c>
       <c r="J25" t="s">
         <v>29</v>
@@ -7258,7 +7256,7 @@
         <v>3</v>
       </c>
       <c r="I32" s="13" t="s">
-        <v>1450</v>
+        <v>1449</v>
       </c>
       <c r="J32" t="s">
         <v>43</v>
@@ -7417,7 +7415,7 @@
         <v>29</v>
       </c>
       <c r="K35" t="s">
-        <v>1432</v>
+        <v>1431</v>
       </c>
       <c r="M35">
         <v>1</v>
@@ -7468,7 +7466,7 @@
         <v>29</v>
       </c>
       <c r="K36" t="s">
-        <v>1432</v>
+        <v>1431</v>
       </c>
       <c r="M36">
         <v>2</v>
@@ -7519,7 +7517,7 @@
         <v>29</v>
       </c>
       <c r="K37" t="s">
-        <v>1432</v>
+        <v>1431</v>
       </c>
       <c r="M37">
         <v>3</v>
@@ -7567,7 +7565,7 @@
         <v>3</v>
       </c>
       <c r="I38" t="s">
-        <v>1447</v>
+        <v>1446</v>
       </c>
       <c r="J38" t="s">
         <v>21</v>
@@ -7620,7 +7618,7 @@
         <v>3</v>
       </c>
       <c r="I39" t="s">
-        <v>1447</v>
+        <v>1446</v>
       </c>
       <c r="J39" t="s">
         <v>29</v>
@@ -7673,7 +7671,7 @@
         <v>3</v>
       </c>
       <c r="I40" t="s">
-        <v>1447</v>
+        <v>1446</v>
       </c>
       <c r="J40" t="s">
         <v>21</v>
@@ -7726,7 +7724,7 @@
         <v>3</v>
       </c>
       <c r="I41" t="s">
-        <v>1447</v>
+        <v>1446</v>
       </c>
       <c r="J41" t="s">
         <v>21</v>
@@ -7779,7 +7777,7 @@
         <v>3</v>
       </c>
       <c r="I42" t="s">
-        <v>1447</v>
+        <v>1446</v>
       </c>
       <c r="J42" t="s">
         <v>29</v>
@@ -7832,7 +7830,7 @@
         <v>3</v>
       </c>
       <c r="I43" t="s">
-        <v>1447</v>
+        <v>1446</v>
       </c>
       <c r="J43" t="s">
         <v>21</v>
@@ -7885,7 +7883,7 @@
         <v>3</v>
       </c>
       <c r="I44" t="s">
-        <v>1447</v>
+        <v>1446</v>
       </c>
       <c r="J44" t="s">
         <v>21</v>
@@ -7938,7 +7936,7 @@
         <v>3</v>
       </c>
       <c r="I45" t="s">
-        <v>1447</v>
+        <v>1446</v>
       </c>
       <c r="J45" t="s">
         <v>29</v>
@@ -7991,7 +7989,7 @@
         <v>3</v>
       </c>
       <c r="I46" t="s">
-        <v>1447</v>
+        <v>1446</v>
       </c>
       <c r="J46" t="s">
         <v>21</v>
@@ -8044,7 +8042,7 @@
         <v>3</v>
       </c>
       <c r="I47" t="s">
-        <v>1447</v>
+        <v>1446</v>
       </c>
       <c r="J47" t="s">
         <v>29</v>
@@ -8100,7 +8098,7 @@
         <v>3</v>
       </c>
       <c r="I48" t="s">
-        <v>1447</v>
+        <v>1446</v>
       </c>
       <c r="J48" t="s">
         <v>29</v>
@@ -8156,7 +8154,7 @@
         <v>3</v>
       </c>
       <c r="I49" t="s">
-        <v>1447</v>
+        <v>1446</v>
       </c>
       <c r="J49" t="s">
         <v>29</v>
@@ -8212,7 +8210,7 @@
         <v>3</v>
       </c>
       <c r="I50" t="s">
-        <v>1447</v>
+        <v>1446</v>
       </c>
       <c r="J50" t="s">
         <v>29</v>
@@ -8268,7 +8266,7 @@
         <v>3</v>
       </c>
       <c r="I51" t="s">
-        <v>1447</v>
+        <v>1446</v>
       </c>
       <c r="J51" t="s">
         <v>29</v>
@@ -8324,7 +8322,7 @@
         <v>3</v>
       </c>
       <c r="I52" t="s">
-        <v>1447</v>
+        <v>1446</v>
       </c>
       <c r="J52" t="s">
         <v>29</v>
@@ -8380,7 +8378,7 @@
         <v>3</v>
       </c>
       <c r="I53" t="s">
-        <v>1447</v>
+        <v>1446</v>
       </c>
       <c r="J53" t="s">
         <v>29</v>
@@ -8436,7 +8434,7 @@
         <v>3</v>
       </c>
       <c r="I54" t="s">
-        <v>1447</v>
+        <v>1446</v>
       </c>
       <c r="J54" t="s">
         <v>29</v>
@@ -9187,13 +9185,13 @@
         <v>3</v>
       </c>
       <c r="I68" s="14" t="s">
-        <v>1447</v>
+        <v>1446</v>
       </c>
       <c r="J68" t="s">
-        <v>1435</v>
+        <v>1434</v>
       </c>
       <c r="K68" t="s">
-        <v>1434</v>
+        <v>1433</v>
       </c>
       <c r="M68">
         <v>1</v>
@@ -9240,13 +9238,13 @@
         <v>3</v>
       </c>
       <c r="I69" s="14" t="s">
-        <v>1447</v>
+        <v>1446</v>
       </c>
       <c r="J69" t="s">
-        <v>1435</v>
+        <v>1434</v>
       </c>
       <c r="K69" t="s">
-        <v>1434</v>
+        <v>1433</v>
       </c>
       <c r="M69">
         <v>2</v>
@@ -9293,13 +9291,13 @@
         <v>3</v>
       </c>
       <c r="I70" s="14" t="s">
-        <v>1447</v>
+        <v>1446</v>
       </c>
       <c r="J70" t="s">
-        <v>1435</v>
+        <v>1434</v>
       </c>
       <c r="K70" t="s">
-        <v>1434</v>
+        <v>1433</v>
       </c>
       <c r="M70">
         <v>3</v>
@@ -9346,7 +9344,7 @@
         <v>3</v>
       </c>
       <c r="I71" s="14" t="s">
-        <v>1447</v>
+        <v>1446</v>
       </c>
       <c r="J71" t="s">
         <v>29</v>
@@ -9399,7 +9397,7 @@
         <v>3</v>
       </c>
       <c r="I72" s="14" t="s">
-        <v>1447</v>
+        <v>1446</v>
       </c>
       <c r="J72" t="s">
         <v>29</v>
@@ -9452,7 +9450,7 @@
         <v>3</v>
       </c>
       <c r="I73" s="14" t="s">
-        <v>1447</v>
+        <v>1446</v>
       </c>
       <c r="J73" t="s">
         <v>29</v>
@@ -9505,13 +9503,13 @@
         <v>3</v>
       </c>
       <c r="I74" s="14" t="s">
-        <v>1448</v>
+        <v>1447</v>
       </c>
       <c r="J74" t="s">
-        <v>1435</v>
+        <v>1434</v>
       </c>
       <c r="K74" t="s">
-        <v>1433</v>
+        <v>1432</v>
       </c>
       <c r="M74">
         <v>1</v>
@@ -9558,13 +9556,13 @@
         <v>3</v>
       </c>
       <c r="I75" s="14" t="s">
-        <v>1448</v>
+        <v>1447</v>
       </c>
       <c r="J75" t="s">
-        <v>1435</v>
+        <v>1434</v>
       </c>
       <c r="K75" t="s">
-        <v>1433</v>
+        <v>1432</v>
       </c>
       <c r="M75">
         <v>2</v>
@@ -9611,13 +9609,13 @@
         <v>3</v>
       </c>
       <c r="I76" s="14" t="s">
-        <v>1448</v>
+        <v>1447</v>
       </c>
       <c r="J76" t="s">
-        <v>1435</v>
+        <v>1434</v>
       </c>
       <c r="K76" t="s">
-        <v>1433</v>
+        <v>1432</v>
       </c>
       <c r="M76">
         <v>3</v>
@@ -9664,7 +9662,7 @@
         <v>3</v>
       </c>
       <c r="I77" s="14" t="s">
-        <v>1448</v>
+        <v>1447</v>
       </c>
       <c r="J77" t="s">
         <v>29</v>
@@ -9717,7 +9715,7 @@
         <v>3</v>
       </c>
       <c r="I78" s="14" t="s">
-        <v>1448</v>
+        <v>1447</v>
       </c>
       <c r="J78" t="s">
         <v>29</v>
@@ -9770,7 +9768,7 @@
         <v>3</v>
       </c>
       <c r="I79" s="14" t="s">
-        <v>1448</v>
+        <v>1447</v>
       </c>
       <c r="J79" t="s">
         <v>29</v>
@@ -9824,7 +9822,7 @@
       </c>
       <c r="I80" s="14"/>
       <c r="J80" t="s">
-        <v>1435</v>
+        <v>1434</v>
       </c>
       <c r="K80" t="s">
         <v>76</v>
@@ -9848,7 +9846,7 @@
         <v>193</v>
       </c>
       <c r="S80" s="8" t="s">
-        <v>1419</v>
+        <v>1418</v>
       </c>
     </row>
     <row r="81" spans="1:19">
@@ -9878,7 +9876,7 @@
       </c>
       <c r="I81" s="14"/>
       <c r="J81" t="s">
-        <v>1435</v>
+        <v>1434</v>
       </c>
       <c r="K81" t="s">
         <v>76</v>
@@ -9902,7 +9900,7 @@
         <v>193</v>
       </c>
       <c r="S81" s="8" t="s">
-        <v>1419</v>
+        <v>1418</v>
       </c>
     </row>
     <row r="82" spans="1:19">
@@ -9932,7 +9930,7 @@
       </c>
       <c r="I82" s="14"/>
       <c r="J82" t="s">
-        <v>1435</v>
+        <v>1434</v>
       </c>
       <c r="K82" t="s">
         <v>76</v>
@@ -9956,7 +9954,7 @@
         <v>193</v>
       </c>
       <c r="S82" s="8" t="s">
-        <v>1419</v>
+        <v>1418</v>
       </c>
     </row>
     <row r="83" spans="1:19">
@@ -10010,7 +10008,7 @@
         <v>188</v>
       </c>
       <c r="S83" s="8" t="s">
-        <v>1420</v>
+        <v>1419</v>
       </c>
     </row>
     <row r="84" spans="1:19">
@@ -10064,7 +10062,7 @@
         <v>188</v>
       </c>
       <c r="S84" s="8" t="s">
-        <v>1420</v>
+        <v>1419</v>
       </c>
     </row>
     <row r="85" spans="1:19">
@@ -10118,7 +10116,7 @@
         <v>188</v>
       </c>
       <c r="S85" s="8" t="s">
-        <v>1420</v>
+        <v>1419</v>
       </c>
     </row>
     <row r="86" spans="1:19">
@@ -10126,7 +10124,7 @@
         <v>17</v>
       </c>
       <c r="C86" t="s">
-        <v>1401</v>
+        <v>1469</v>
       </c>
       <c r="D86" s="3" t="s">
         <v>25</v>
@@ -10138,13 +10136,13 @@
         <v>2016</v>
       </c>
       <c r="G86" t="s">
-        <v>1402</v>
+        <v>1401</v>
       </c>
       <c r="H86">
         <v>4</v>
       </c>
       <c r="I86" s="14" t="s">
-        <v>1447</v>
+        <v>1446</v>
       </c>
       <c r="J86" s="14" t="s">
         <v>29</v>
@@ -10176,7 +10174,7 @@
         <v>17</v>
       </c>
       <c r="C87" t="s">
-        <v>1401</v>
+        <v>1469</v>
       </c>
       <c r="D87" s="3" t="s">
         <v>25</v>
@@ -10188,13 +10186,13 @@
         <v>2016</v>
       </c>
       <c r="G87" t="s">
-        <v>1402</v>
+        <v>1401</v>
       </c>
       <c r="H87">
         <v>4</v>
       </c>
       <c r="I87" s="14" t="s">
-        <v>1447</v>
+        <v>1446</v>
       </c>
       <c r="J87" s="14" t="s">
         <v>29</v>
@@ -10226,7 +10224,7 @@
         <v>17</v>
       </c>
       <c r="C88" t="s">
-        <v>1401</v>
+        <v>1469</v>
       </c>
       <c r="D88" s="3" t="s">
         <v>25</v>
@@ -10238,13 +10236,13 @@
         <v>2016</v>
       </c>
       <c r="G88" t="s">
-        <v>1402</v>
+        <v>1401</v>
       </c>
       <c r="H88">
         <v>4</v>
       </c>
       <c r="I88" s="14" t="s">
-        <v>1447</v>
+        <v>1446</v>
       </c>
       <c r="J88" s="14" t="s">
         <v>29</v>
@@ -10276,7 +10274,7 @@
         <v>17</v>
       </c>
       <c r="C89" t="s">
-        <v>1401</v>
+        <v>1469</v>
       </c>
       <c r="D89" s="3" t="s">
         <v>25</v>
@@ -10288,13 +10286,13 @@
         <v>2016</v>
       </c>
       <c r="G89" t="s">
-        <v>1402</v>
+        <v>1401</v>
       </c>
       <c r="H89">
         <v>4</v>
       </c>
       <c r="I89" s="14" t="s">
-        <v>1447</v>
+        <v>1446</v>
       </c>
       <c r="J89" t="s">
         <v>21</v>
@@ -10326,7 +10324,7 @@
         <v>17</v>
       </c>
       <c r="C90" t="s">
-        <v>1401</v>
+        <v>1469</v>
       </c>
       <c r="D90" s="3" t="s">
         <v>25</v>
@@ -10338,13 +10336,13 @@
         <v>2016</v>
       </c>
       <c r="G90" t="s">
-        <v>1402</v>
+        <v>1401</v>
       </c>
       <c r="H90">
         <v>4</v>
       </c>
       <c r="I90" s="14" t="s">
-        <v>1447</v>
+        <v>1446</v>
       </c>
       <c r="J90" t="s">
         <v>21</v>
@@ -10376,7 +10374,7 @@
         <v>17</v>
       </c>
       <c r="C91" t="s">
-        <v>1401</v>
+        <v>1469</v>
       </c>
       <c r="D91" s="3" t="s">
         <v>25</v>
@@ -10388,13 +10386,13 @@
         <v>2016</v>
       </c>
       <c r="G91" t="s">
-        <v>1402</v>
+        <v>1401</v>
       </c>
       <c r="H91">
         <v>4</v>
       </c>
       <c r="I91" s="14" t="s">
-        <v>1447</v>
+        <v>1446</v>
       </c>
       <c r="J91" t="s">
         <v>21</v>
@@ -10426,13 +10424,13 @@
         <v>114</v>
       </c>
       <c r="C92" t="s">
-        <v>1427</v>
+        <v>1426</v>
       </c>
       <c r="D92" s="3" t="s">
-        <v>1426</v>
+        <v>1425</v>
       </c>
       <c r="E92" t="s">
-        <v>1431</v>
+        <v>1430</v>
       </c>
       <c r="F92" s="3">
         <v>2025</v>
@@ -10448,7 +10446,7 @@
         <v>21</v>
       </c>
       <c r="K92" t="s">
-        <v>1428</v>
+        <v>1427</v>
       </c>
       <c r="M92">
         <v>1</v>
@@ -10474,13 +10472,13 @@
         <v>114</v>
       </c>
       <c r="C93" t="s">
-        <v>1427</v>
+        <v>1426</v>
       </c>
       <c r="D93" s="3" t="s">
-        <v>1426</v>
+        <v>1425</v>
       </c>
       <c r="E93" t="s">
-        <v>1431</v>
+        <v>1430</v>
       </c>
       <c r="F93" s="3">
         <v>2025</v>
@@ -10496,7 +10494,7 @@
         <v>21</v>
       </c>
       <c r="K93" t="s">
-        <v>1428</v>
+        <v>1427</v>
       </c>
       <c r="M93">
         <v>2</v>
@@ -10522,13 +10520,13 @@
         <v>114</v>
       </c>
       <c r="C94" t="s">
-        <v>1427</v>
+        <v>1426</v>
       </c>
       <c r="D94" s="3" t="s">
-        <v>1426</v>
+        <v>1425</v>
       </c>
       <c r="E94" t="s">
-        <v>1431</v>
+        <v>1430</v>
       </c>
       <c r="F94" s="3">
         <v>2025</v>
@@ -10544,7 +10542,7 @@
         <v>21</v>
       </c>
       <c r="K94" t="s">
-        <v>1428</v>
+        <v>1427</v>
       </c>
       <c r="M94">
         <v>3</v>
@@ -10570,19 +10568,19 @@
         <v>114</v>
       </c>
       <c r="C95" t="s">
-        <v>1427</v>
+        <v>1426</v>
       </c>
       <c r="D95" s="3" t="s">
-        <v>1426</v>
+        <v>1425</v>
       </c>
       <c r="E95" t="s">
-        <v>1431</v>
+        <v>1430</v>
       </c>
       <c r="F95" s="3">
         <v>2025</v>
       </c>
       <c r="G95" t="s">
-        <v>1429</v>
+        <v>1428</v>
       </c>
       <c r="H95">
         <v>4</v>
@@ -10592,7 +10590,7 @@
         <v>21</v>
       </c>
       <c r="K95" t="s">
-        <v>1428</v>
+        <v>1427</v>
       </c>
       <c r="M95">
         <v>1</v>
@@ -10613,7 +10611,7 @@
         <v>102</v>
       </c>
       <c r="S95" t="s">
-        <v>1430</v>
+        <v>1429</v>
       </c>
     </row>
     <row r="96" spans="1:19">
@@ -10621,19 +10619,19 @@
         <v>114</v>
       </c>
       <c r="C96" t="s">
-        <v>1427</v>
+        <v>1426</v>
       </c>
       <c r="D96" s="3" t="s">
-        <v>1426</v>
+        <v>1425</v>
       </c>
       <c r="E96" t="s">
-        <v>1431</v>
+        <v>1430</v>
       </c>
       <c r="F96" s="3">
         <v>2025</v>
       </c>
       <c r="G96" t="s">
-        <v>1429</v>
+        <v>1428</v>
       </c>
       <c r="H96">
         <v>4</v>
@@ -10643,7 +10641,7 @@
         <v>21</v>
       </c>
       <c r="K96" t="s">
-        <v>1428</v>
+        <v>1427</v>
       </c>
       <c r="M96">
         <v>2</v>
@@ -10664,7 +10662,7 @@
         <v>102</v>
       </c>
       <c r="S96" t="s">
-        <v>1430</v>
+        <v>1429</v>
       </c>
     </row>
     <row r="97" spans="1:19">
@@ -10672,19 +10670,19 @@
         <v>114</v>
       </c>
       <c r="C97" t="s">
-        <v>1427</v>
+        <v>1426</v>
       </c>
       <c r="D97" s="3" t="s">
-        <v>1426</v>
+        <v>1425</v>
       </c>
       <c r="E97" t="s">
-        <v>1431</v>
+        <v>1430</v>
       </c>
       <c r="F97" s="3">
         <v>2025</v>
       </c>
       <c r="G97" t="s">
-        <v>1429</v>
+        <v>1428</v>
       </c>
       <c r="H97">
         <v>4</v>
@@ -10694,7 +10692,7 @@
         <v>21</v>
       </c>
       <c r="K97" t="s">
-        <v>1428</v>
+        <v>1427</v>
       </c>
       <c r="M97">
         <v>3</v>
@@ -10715,7 +10713,7 @@
         <v>102</v>
       </c>
       <c r="S97" t="s">
-        <v>1430</v>
+        <v>1429</v>
       </c>
     </row>
     <row r="1048575" spans="7:7">
@@ -10734,7 +10732,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B357E3A0-CAC3-4594-9484-B64331912218}">
   <dimension ref="A1:X33"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="4" ySplit="1" topLeftCell="E2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
@@ -10743,36 +10741,33 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="8.7265625" style="16"/>
-    <col min="2" max="2" width="13.54296875" style="16" customWidth="1"/>
-    <col min="3" max="3" width="28.1796875" style="16" customWidth="1"/>
-    <col min="4" max="5" width="30.36328125" style="16" customWidth="1"/>
-    <col min="6" max="6" width="15.36328125" style="16" customWidth="1"/>
-    <col min="7" max="7" width="16.6328125" style="16" customWidth="1"/>
-    <col min="8" max="8" width="17.453125" style="16" customWidth="1"/>
-    <col min="9" max="9" width="8.7265625" style="16"/>
-    <col min="10" max="10" width="36.54296875" style="16" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="42.81640625" style="16" customWidth="1"/>
-    <col min="12" max="16384" width="8.7265625" style="16"/>
+    <col min="2" max="2" width="13.54296875" customWidth="1"/>
+    <col min="3" max="3" width="28.1796875" customWidth="1"/>
+    <col min="4" max="5" width="30.36328125" customWidth="1"/>
+    <col min="6" max="6" width="15.36328125" customWidth="1"/>
+    <col min="7" max="7" width="16.6328125" customWidth="1"/>
+    <col min="8" max="8" width="17.453125" customWidth="1"/>
+    <col min="10" max="10" width="36.54296875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="42.81640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11">
-      <c r="A1" s="16" t="s">
-        <v>1425</v>
-      </c>
-      <c r="B1" s="16" t="s">
+      <c r="A1" t="s">
+        <v>1424</v>
+      </c>
+      <c r="B1" t="s">
         <v>79</v>
       </c>
-      <c r="C1" s="16" t="s">
+      <c r="C1" t="s">
         <v>80</v>
       </c>
-      <c r="D1" s="16" t="s">
+      <c r="D1" t="s">
         <v>81</v>
       </c>
-      <c r="E1" s="16" t="s">
-        <v>1446</v>
-      </c>
-      <c r="F1" s="16" t="s">
+      <c r="E1" t="s">
+        <v>1445</v>
+      </c>
+      <c r="F1" t="s">
         <v>1375</v>
       </c>
       <c r="G1" s="8" t="s">
@@ -10784,7 +10779,7 @@
       <c r="I1" s="8" t="s">
         <v>84</v>
       </c>
-      <c r="J1" s="16" t="s">
+      <c r="J1" t="s">
         <v>16</v>
       </c>
       <c r="K1" s="12" t="s">
@@ -10792,1062 +10787,1062 @@
       </c>
     </row>
     <row r="2" spans="1:11">
-      <c r="A2" s="16">
+      <c r="A2">
         <v>103</v>
       </c>
-      <c r="B2" s="16" t="s">
+      <c r="B2" t="s">
         <v>86</v>
       </c>
-      <c r="C2" s="16" t="s">
+      <c r="C2" t="s">
         <v>87</v>
       </c>
-      <c r="D2" s="16" t="s">
+      <c r="D2" t="s">
         <v>88</v>
       </c>
-      <c r="E2" s="16" t="s">
+      <c r="E2" t="s">
+        <v>1464</v>
+      </c>
+      <c r="G2" t="s">
+        <v>15</v>
+      </c>
+      <c r="H2">
+        <v>0</v>
+      </c>
+      <c r="I2" t="s">
+        <v>23</v>
+      </c>
+      <c r="J2" t="s">
+        <v>1412</v>
+      </c>
+      <c r="K2" t="s">
+        <v>1373</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11">
+      <c r="A3">
+        <v>11</v>
+      </c>
+      <c r="B3" t="s">
+        <v>86</v>
+      </c>
+      <c r="C3" t="s">
+        <v>89</v>
+      </c>
+      <c r="D3" t="s">
+        <v>90</v>
+      </c>
+      <c r="F3" t="s">
+        <v>135</v>
+      </c>
+      <c r="G3" t="s">
+        <v>23</v>
+      </c>
+      <c r="H3">
+        <v>0</v>
+      </c>
+      <c r="I3" t="s">
+        <v>23</v>
+      </c>
+      <c r="J3" t="s">
+        <v>1408</v>
+      </c>
+      <c r="K3" s="15" t="s">
+        <v>1380</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>86</v>
+      </c>
+      <c r="C4" t="s">
+        <v>91</v>
+      </c>
+      <c r="D4" t="s">
+        <v>92</v>
+      </c>
+      <c r="E4" t="s">
+        <v>1463</v>
+      </c>
+      <c r="F4" t="s">
+        <v>135</v>
+      </c>
+      <c r="G4" t="s">
+        <v>15</v>
+      </c>
+      <c r="H4">
+        <v>0</v>
+      </c>
+      <c r="I4" t="s">
+        <v>23</v>
+      </c>
+      <c r="J4" t="s">
+        <v>1413</v>
+      </c>
+      <c r="K4" s="15" t="s">
+        <v>1376</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11">
+      <c r="A5">
+        <v>5</v>
+      </c>
+      <c r="B5" t="s">
+        <v>86</v>
+      </c>
+      <c r="C5" t="s">
+        <v>93</v>
+      </c>
+      <c r="D5" t="s">
+        <v>94</v>
+      </c>
+      <c r="E5" t="s">
+        <v>1462</v>
+      </c>
+      <c r="F5" t="s">
+        <v>135</v>
+      </c>
+      <c r="G5" t="s">
+        <v>15</v>
+      </c>
+      <c r="H5">
+        <v>0</v>
+      </c>
+      <c r="I5" t="s">
+        <v>23</v>
+      </c>
+      <c r="J5" t="s">
+        <v>1415</v>
+      </c>
+      <c r="K5" s="15" t="s">
+        <v>1381</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11">
+      <c r="A6">
+        <v>9</v>
+      </c>
+      <c r="B6" t="s">
+        <v>86</v>
+      </c>
+      <c r="C6" t="s">
+        <v>95</v>
+      </c>
+      <c r="D6" t="s">
+        <v>96</v>
+      </c>
+      <c r="E6" t="s">
+        <v>1458</v>
+      </c>
+      <c r="F6" t="s">
+        <v>135</v>
+      </c>
+      <c r="G6" t="s">
+        <v>15</v>
+      </c>
+      <c r="H6">
+        <v>0</v>
+      </c>
+      <c r="I6" t="s">
+        <v>23</v>
+      </c>
+      <c r="J6" t="s">
+        <v>1411</v>
+      </c>
+      <c r="K6" t="s">
+        <v>1416</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11">
+      <c r="A7">
+        <v>13</v>
+      </c>
+      <c r="B7" t="s">
+        <v>86</v>
+      </c>
+      <c r="C7" t="s">
+        <v>97</v>
+      </c>
+      <c r="D7" t="s">
+        <v>98</v>
+      </c>
+      <c r="F7" t="s">
+        <v>135</v>
+      </c>
+      <c r="G7" t="s">
+        <v>15</v>
+      </c>
+      <c r="H7">
+        <v>0</v>
+      </c>
+      <c r="I7" t="s">
+        <v>23</v>
+      </c>
+      <c r="J7" t="s">
+        <v>1414</v>
+      </c>
+      <c r="K7" t="s">
+        <v>1378</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11">
+      <c r="A8">
+        <v>17</v>
+      </c>
+      <c r="B8" t="s">
+        <v>86</v>
+      </c>
+      <c r="C8" t="s">
+        <v>99</v>
+      </c>
+      <c r="D8" t="s">
+        <v>100</v>
+      </c>
+      <c r="E8" s="14" t="s">
+        <v>1446</v>
+      </c>
+      <c r="F8" t="s">
+        <v>1402</v>
+      </c>
+      <c r="G8" t="s">
+        <v>15</v>
+      </c>
+      <c r="H8">
+        <v>0</v>
+      </c>
+      <c r="I8" t="s">
+        <v>23</v>
+      </c>
+      <c r="J8" t="s">
+        <v>1406</v>
+      </c>
+      <c r="K8" s="15" t="s">
+        <v>1400</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11">
+      <c r="A9">
+        <v>23</v>
+      </c>
+      <c r="B9" t="s">
+        <v>86</v>
+      </c>
+      <c r="C9" t="s">
+        <v>99</v>
+      </c>
+      <c r="D9" t="s">
+        <v>101</v>
+      </c>
+      <c r="E9" t="s">
+        <v>1468</v>
+      </c>
+      <c r="F9" t="s">
+        <v>1410</v>
+      </c>
+      <c r="G9" t="s">
+        <v>23</v>
+      </c>
+      <c r="H9">
+        <v>0</v>
+      </c>
+      <c r="I9" t="s">
+        <v>23</v>
+      </c>
+      <c r="J9" t="s">
+        <v>1407</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11">
+      <c r="A10">
+        <v>106</v>
+      </c>
+      <c r="B10" t="s">
+        <v>86</v>
+      </c>
+      <c r="C10" t="s">
+        <v>102</v>
+      </c>
+      <c r="D10" t="s">
+        <v>103</v>
+      </c>
+      <c r="E10" t="s">
+        <v>1449</v>
+      </c>
+      <c r="F10" t="s">
+        <v>135</v>
+      </c>
+      <c r="G10" t="s">
+        <v>23</v>
+      </c>
+      <c r="H10" t="s">
+        <v>23</v>
+      </c>
+      <c r="I10" t="s">
+        <v>23</v>
+      </c>
+      <c r="J10" t="s">
+        <v>1409</v>
+      </c>
+      <c r="K10" t="s">
+        <v>1377</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11">
+      <c r="A11">
+        <v>108</v>
+      </c>
+      <c r="B11" t="s">
+        <v>86</v>
+      </c>
+      <c r="C11" t="s">
+        <v>104</v>
+      </c>
+      <c r="D11" t="s">
+        <v>105</v>
+      </c>
+      <c r="E11" t="s">
+        <v>1446</v>
+      </c>
+      <c r="F11" t="s">
+        <v>135</v>
+      </c>
+      <c r="G11" t="s">
+        <v>15</v>
+      </c>
+      <c r="H11">
+        <v>0</v>
+      </c>
+      <c r="I11" t="s">
+        <v>23</v>
+      </c>
+      <c r="J11" t="s">
+        <v>1405</v>
+      </c>
+      <c r="K11" s="15" t="s">
+        <v>1374</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11">
+      <c r="A12">
+        <v>110</v>
+      </c>
+      <c r="B12" t="s">
+        <v>106</v>
+      </c>
+      <c r="C12" t="s">
+        <v>107</v>
+      </c>
+      <c r="D12" t="s">
+        <v>108</v>
+      </c>
+      <c r="E12" t="s">
+        <v>1466</v>
+      </c>
+      <c r="F12" t="s">
+        <v>135</v>
+      </c>
+      <c r="G12" t="s">
+        <v>15</v>
+      </c>
+      <c r="H12">
+        <v>0</v>
+      </c>
+      <c r="I12" t="s">
+        <v>23</v>
+      </c>
+      <c r="J12" t="s">
+        <v>1421</v>
+      </c>
+      <c r="K12" t="s">
+        <v>1073</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11">
+      <c r="A13">
+        <v>1</v>
+      </c>
+      <c r="B13" t="s">
+        <v>106</v>
+      </c>
+      <c r="C13" t="s">
+        <v>109</v>
+      </c>
+      <c r="D13" t="s">
+        <v>110</v>
+      </c>
+      <c r="F13" t="s">
+        <v>135</v>
+      </c>
+      <c r="G13" t="s">
+        <v>15</v>
+      </c>
+      <c r="H13">
+        <v>0</v>
+      </c>
+      <c r="I13" t="s">
+        <v>23</v>
+      </c>
+      <c r="K13" t="s">
+        <v>1379</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11">
+      <c r="A14">
+        <v>8</v>
+      </c>
+      <c r="B14" t="s">
+        <v>106</v>
+      </c>
+      <c r="C14" t="s">
+        <v>111</v>
+      </c>
+      <c r="D14" t="s">
+        <v>112</v>
+      </c>
+      <c r="E14" t="s">
+        <v>1458</v>
+      </c>
+      <c r="F14" t="s">
+        <v>135</v>
+      </c>
+      <c r="G14" t="s">
+        <v>15</v>
+      </c>
+      <c r="H14">
+        <v>2</v>
+      </c>
+      <c r="I14" t="s">
+        <v>145</v>
+      </c>
+      <c r="J14" t="s">
+        <v>1383</v>
+      </c>
+      <c r="K14" t="s">
+        <v>1382</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11">
+      <c r="A15">
+        <v>105</v>
+      </c>
+      <c r="B15" t="s">
+        <v>106</v>
+      </c>
+      <c r="C15" t="s">
+        <v>113</v>
+      </c>
+      <c r="D15" t="s">
+        <v>114</v>
+      </c>
+      <c r="F15" t="s">
+        <v>135</v>
+      </c>
+      <c r="G15" t="s">
+        <v>15</v>
+      </c>
+      <c r="H15">
+        <v>0</v>
+      </c>
+      <c r="I15" t="s">
+        <v>23</v>
+      </c>
+      <c r="J15" t="s">
+        <v>1385</v>
+      </c>
+      <c r="K15" t="s">
+        <v>1384</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11">
+      <c r="A16">
+        <v>19</v>
+      </c>
+      <c r="B16" t="s">
+        <v>106</v>
+      </c>
+      <c r="C16" t="s">
+        <v>115</v>
+      </c>
+      <c r="D16" t="s">
+        <v>116</v>
+      </c>
+      <c r="F16" t="s">
+        <v>135</v>
+      </c>
+      <c r="G16" t="s">
+        <v>15</v>
+      </c>
+      <c r="H16">
+        <v>2</v>
+      </c>
+      <c r="I16" t="s">
+        <v>145</v>
+      </c>
+      <c r="J16" t="s">
+        <v>1387</v>
+      </c>
+      <c r="K16" t="s">
+        <v>1388</v>
+      </c>
+    </row>
+    <row r="17" spans="1:24">
+      <c r="A17">
+        <v>25</v>
+      </c>
+      <c r="B17" t="s">
+        <v>106</v>
+      </c>
+      <c r="C17" t="s">
+        <v>117</v>
+      </c>
+      <c r="D17" t="s">
+        <v>118</v>
+      </c>
+      <c r="E17" t="s">
         <v>1465</v>
       </c>
-      <c r="G2" s="16" t="s">
+      <c r="F17" t="s">
+        <v>135</v>
+      </c>
+      <c r="G17" t="s">
         <v>15</v>
       </c>
-      <c r="H2" s="16">
+      <c r="H17">
+        <v>1</v>
+      </c>
+      <c r="I17" t="s">
+        <v>1390</v>
+      </c>
+      <c r="J17" t="s">
+        <v>1404</v>
+      </c>
+      <c r="K17" t="s">
+        <v>1389</v>
+      </c>
+      <c r="X17" s="16" t="s">
+        <v>1403</v>
+      </c>
+    </row>
+    <row r="18" spans="1:24">
+      <c r="A18">
+        <v>26</v>
+      </c>
+      <c r="B18" t="s">
+        <v>106</v>
+      </c>
+      <c r="C18" t="s">
+        <v>119</v>
+      </c>
+      <c r="D18" t="s">
+        <v>120</v>
+      </c>
+      <c r="F18" t="s">
+        <v>135</v>
+      </c>
+      <c r="G18" t="s">
+        <v>15</v>
+      </c>
+      <c r="H18">
         <v>0</v>
       </c>
-      <c r="I2" s="16" t="s">
+      <c r="I18" t="s">
         <v>23</v>
       </c>
-      <c r="J2" s="16" t="s">
-        <v>1413</v>
-      </c>
-      <c r="K2" s="16" t="s">
-        <v>1373</v>
-      </c>
-    </row>
-    <row r="3" spans="1:11">
-      <c r="A3" s="16">
-        <v>11</v>
-      </c>
-      <c r="B3" s="16" t="s">
-        <v>86</v>
-      </c>
-      <c r="C3" s="16" t="s">
-        <v>89</v>
-      </c>
-      <c r="D3" s="16" t="s">
-        <v>90</v>
-      </c>
-      <c r="F3" s="16" t="s">
+      <c r="K18" t="s">
+        <v>1391</v>
+      </c>
+    </row>
+    <row r="19" spans="1:24">
+      <c r="A19">
+        <v>7</v>
+      </c>
+      <c r="B19" t="s">
+        <v>106</v>
+      </c>
+      <c r="C19" t="s">
+        <v>121</v>
+      </c>
+      <c r="D19" t="s">
+        <v>122</v>
+      </c>
+      <c r="F19" t="s">
         <v>135</v>
       </c>
-      <c r="G3" s="16" t="s">
+      <c r="G19" t="s">
+        <v>15</v>
+      </c>
+      <c r="H19">
+        <v>1</v>
+      </c>
+      <c r="I19" t="s">
+        <v>145</v>
+      </c>
+      <c r="J19" t="s">
+        <v>1392</v>
+      </c>
+      <c r="K19" t="s">
+        <v>618</v>
+      </c>
+    </row>
+    <row r="20" spans="1:24">
+      <c r="A20">
+        <v>14</v>
+      </c>
+      <c r="B20" t="s">
+        <v>106</v>
+      </c>
+      <c r="C20" t="s">
+        <v>123</v>
+      </c>
+      <c r="D20" t="s">
+        <v>124</v>
+      </c>
+      <c r="E20" t="s">
+        <v>1461</v>
+      </c>
+      <c r="F20" s="14" t="s">
+        <v>15</v>
+      </c>
+      <c r="G20" t="s">
+        <v>15</v>
+      </c>
+      <c r="H20">
+        <v>0</v>
+      </c>
+      <c r="I20" t="s">
         <v>23</v>
       </c>
-      <c r="H3" s="16">
+      <c r="J20" t="s">
+        <v>1422</v>
+      </c>
+      <c r="K20" t="s">
+        <v>1395</v>
+      </c>
+    </row>
+    <row r="21" spans="1:24" ht="15" customHeight="1">
+      <c r="A21">
+        <v>22</v>
+      </c>
+      <c r="B21" t="s">
+        <v>106</v>
+      </c>
+      <c r="C21" t="s">
+        <v>125</v>
+      </c>
+      <c r="D21" t="s">
+        <v>126</v>
+      </c>
+      <c r="F21" t="s">
+        <v>135</v>
+      </c>
+      <c r="G21" t="s">
+        <v>15</v>
+      </c>
+      <c r="H21">
         <v>0</v>
       </c>
-      <c r="I3" s="16" t="s">
+      <c r="I21" t="s">
         <v>23</v>
       </c>
-      <c r="J3" s="16" t="s">
-        <v>1409</v>
-      </c>
-      <c r="K3" s="17" t="s">
-        <v>1380</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11">
-      <c r="A4" s="16">
-        <v>3</v>
-      </c>
-      <c r="B4" s="16" t="s">
-        <v>86</v>
-      </c>
-      <c r="C4" s="16" t="s">
-        <v>91</v>
-      </c>
-      <c r="D4" s="16" t="s">
-        <v>92</v>
-      </c>
-      <c r="E4" s="16" t="s">
-        <v>1464</v>
-      </c>
-      <c r="F4" s="16" t="s">
+      <c r="J21" t="s">
+        <v>1399</v>
+      </c>
+      <c r="K21" t="s">
+        <v>1397</v>
+      </c>
+    </row>
+    <row r="22" spans="1:24">
+      <c r="A22">
+        <v>24</v>
+      </c>
+      <c r="B22" t="s">
+        <v>127</v>
+      </c>
+      <c r="C22" t="s">
+        <v>128</v>
+      </c>
+      <c r="D22" t="s">
+        <v>129</v>
+      </c>
+      <c r="F22" t="s">
         <v>135</v>
       </c>
-      <c r="G4" s="16" t="s">
+      <c r="G22" t="s">
         <v>15</v>
       </c>
-      <c r="H4" s="16">
+      <c r="H22">
         <v>0</v>
       </c>
-      <c r="I4" s="16" t="s">
+      <c r="I22" t="s">
         <v>23</v>
       </c>
-      <c r="J4" s="16" t="s">
-        <v>1414</v>
-      </c>
-      <c r="K4" s="17" t="s">
-        <v>1376</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11">
-      <c r="A5" s="16">
-        <v>5</v>
-      </c>
-      <c r="B5" s="16" t="s">
-        <v>86</v>
-      </c>
-      <c r="C5" s="16" t="s">
-        <v>93</v>
-      </c>
-      <c r="D5" s="16" t="s">
-        <v>94</v>
-      </c>
-      <c r="E5" s="16" t="s">
-        <v>1463</v>
-      </c>
-      <c r="F5" s="16" t="s">
+      <c r="K22" t="s">
+        <v>1398</v>
+      </c>
+    </row>
+    <row r="23" spans="1:24" ht="15.5">
+      <c r="A23">
+        <v>27</v>
+      </c>
+      <c r="B23" t="s">
+        <v>127</v>
+      </c>
+      <c r="C23" t="s">
+        <v>130</v>
+      </c>
+      <c r="D23" t="s">
+        <v>131</v>
+      </c>
+      <c r="F23" t="s">
         <v>135</v>
       </c>
-      <c r="G5" s="16" t="s">
+      <c r="G23" t="s">
         <v>15</v>
       </c>
-      <c r="H5" s="16">
+      <c r="H23">
         <v>0</v>
       </c>
-      <c r="I5" s="16" t="s">
+      <c r="I23" t="s">
         <v>23</v>
       </c>
-      <c r="J5" s="16" t="s">
-        <v>1416</v>
-      </c>
-      <c r="K5" s="17" t="s">
-        <v>1381</v>
-      </c>
-    </row>
-    <row r="6" spans="1:11">
-      <c r="A6" s="16">
-        <v>9</v>
-      </c>
-      <c r="B6" s="16" t="s">
-        <v>86</v>
-      </c>
-      <c r="C6" s="16" t="s">
-        <v>95</v>
-      </c>
-      <c r="D6" s="16" t="s">
+      <c r="K23" s="17" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="24" spans="1:24">
+      <c r="A24">
+        <v>28</v>
+      </c>
+      <c r="B24" t="s">
+        <v>127</v>
+      </c>
+      <c r="C24" t="s">
+        <v>133</v>
+      </c>
+      <c r="D24" t="s">
+        <v>134</v>
+      </c>
+      <c r="E24" t="s">
+        <v>1467</v>
+      </c>
+      <c r="F24" t="s">
+        <v>135</v>
+      </c>
+      <c r="G24" t="s">
+        <v>15</v>
+      </c>
+      <c r="H24">
+        <v>0</v>
+      </c>
+      <c r="I24" t="s">
+        <v>23</v>
+      </c>
+      <c r="J24" t="s">
+        <v>1386</v>
+      </c>
+      <c r="K24" s="15" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="25" spans="1:24">
+      <c r="A25">
+        <v>28</v>
+      </c>
+      <c r="B25" t="s">
+        <v>127</v>
+      </c>
+      <c r="C25" t="s">
+        <v>138</v>
+      </c>
+      <c r="D25" t="s">
+        <v>134</v>
+      </c>
+      <c r="E25" t="s">
+        <v>1467</v>
+      </c>
+      <c r="F25" t="s">
+        <v>135</v>
+      </c>
+      <c r="G25" t="s">
+        <v>15</v>
+      </c>
+      <c r="H25">
+        <v>0</v>
+      </c>
+      <c r="I25" t="s">
+        <v>23</v>
+      </c>
+      <c r="J25" t="s">
+        <v>1386</v>
+      </c>
+      <c r="K25" s="15" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="26" spans="1:24" ht="15.5">
+      <c r="A26">
+        <v>102</v>
+      </c>
+      <c r="B26" t="s">
+        <v>127</v>
+      </c>
+      <c r="C26" t="s">
+        <v>139</v>
+      </c>
+      <c r="D26" t="s">
+        <v>140</v>
+      </c>
+      <c r="E26" t="s">
+        <v>1460</v>
+      </c>
+      <c r="F26" t="s">
+        <v>135</v>
+      </c>
+      <c r="G26" t="s">
+        <v>15</v>
+      </c>
+      <c r="H26">
+        <v>0</v>
+      </c>
+      <c r="I26" t="s">
+        <v>23</v>
+      </c>
+      <c r="J26" t="s">
+        <v>142</v>
+      </c>
+      <c r="K26" s="18" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="27" spans="1:24" ht="15.5">
+      <c r="A27">
+        <v>111</v>
+      </c>
+      <c r="B27" t="s">
+        <v>127</v>
+      </c>
+      <c r="C27" t="s">
+        <v>143</v>
+      </c>
+      <c r="D27" t="s">
+        <v>144</v>
+      </c>
+      <c r="E27" t="s">
+        <v>1446</v>
+      </c>
+      <c r="F27" t="s">
+        <v>135</v>
+      </c>
+      <c r="G27" t="s">
+        <v>135</v>
+      </c>
+      <c r="H27">
+        <v>1</v>
+      </c>
+      <c r="I27" t="s">
+        <v>145</v>
+      </c>
+      <c r="J27" t="s">
+        <v>147</v>
+      </c>
+      <c r="K27" s="18" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="28" spans="1:24" ht="15.5">
+      <c r="A28">
+        <v>112</v>
+      </c>
+      <c r="B28" t="s">
+        <v>127</v>
+      </c>
+      <c r="C28" t="s">
+        <v>148</v>
+      </c>
+      <c r="D28" t="s">
         <v>96</v>
       </c>
-      <c r="E6" s="16" t="s">
+      <c r="E28" t="s">
+        <v>1458</v>
+      </c>
+      <c r="F28" t="s">
+        <v>135</v>
+      </c>
+      <c r="G28" t="s">
+        <v>1420</v>
+      </c>
+      <c r="H28">
+        <v>1</v>
+      </c>
+      <c r="I28" t="s">
+        <v>136</v>
+      </c>
+      <c r="K28" s="18" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="29" spans="1:24">
+      <c r="A29">
+        <v>113</v>
+      </c>
+      <c r="B29" t="s">
+        <v>127</v>
+      </c>
+      <c r="C29" t="s">
+        <v>150</v>
+      </c>
+      <c r="D29" t="s">
+        <v>151</v>
+      </c>
+      <c r="E29" t="s">
+        <v>1458</v>
+      </c>
+      <c r="F29" t="s">
+        <v>135</v>
+      </c>
+      <c r="G29" t="s">
+        <v>135</v>
+      </c>
+      <c r="H29">
+        <v>1</v>
+      </c>
+      <c r="I29" t="s">
+        <v>145</v>
+      </c>
+      <c r="K29" t="s">
+        <v>1396</v>
+      </c>
+    </row>
+    <row r="30" spans="1:24">
+      <c r="A30">
+        <v>113</v>
+      </c>
+      <c r="B30" t="s">
+        <v>127</v>
+      </c>
+      <c r="C30" t="s">
+        <v>150</v>
+      </c>
+      <c r="D30" t="s">
+        <v>151</v>
+      </c>
+      <c r="E30" t="s">
+        <v>1458</v>
+      </c>
+      <c r="F30" t="s">
+        <v>1417</v>
+      </c>
+      <c r="G30" t="s">
+        <v>135</v>
+      </c>
+      <c r="H30">
+        <v>4</v>
+      </c>
+      <c r="I30" t="s">
+        <v>145</v>
+      </c>
+      <c r="K30" t="s">
+        <v>1396</v>
+      </c>
+    </row>
+    <row r="31" spans="1:24" ht="15.5">
+      <c r="A31">
+        <v>104</v>
+      </c>
+      <c r="B31" t="s">
+        <v>127</v>
+      </c>
+      <c r="C31" t="s">
+        <v>152</v>
+      </c>
+      <c r="D31" t="s">
+        <v>103</v>
+      </c>
+      <c r="E31" t="s">
         <v>1459</v>
       </c>
-      <c r="F6" s="16" t="s">
+      <c r="F31" t="s">
         <v>135</v>
       </c>
-      <c r="G6" s="16" t="s">
+      <c r="G31" t="s">
         <v>15</v>
       </c>
-      <c r="H6" s="16">
+      <c r="H31">
         <v>0</v>
       </c>
-      <c r="I6" s="16" t="s">
+      <c r="I31" t="s">
         <v>23</v>
       </c>
-      <c r="J6" s="16" t="s">
-        <v>1412</v>
-      </c>
-      <c r="K6" s="16" t="s">
-        <v>1417</v>
-      </c>
-    </row>
-    <row r="7" spans="1:11">
-      <c r="A7" s="16">
-        <v>13</v>
-      </c>
-      <c r="B7" s="16" t="s">
-        <v>86</v>
-      </c>
-      <c r="C7" s="16" t="s">
-        <v>97</v>
-      </c>
-      <c r="D7" s="16" t="s">
-        <v>98</v>
-      </c>
-      <c r="F7" s="16" t="s">
+      <c r="K31" s="18" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="32" spans="1:24" ht="15.5">
+      <c r="A32">
+        <v>107</v>
+      </c>
+      <c r="B32" t="s">
+        <v>127</v>
+      </c>
+      <c r="C32" t="s">
+        <v>154</v>
+      </c>
+      <c r="D32" t="s">
+        <v>155</v>
+      </c>
+      <c r="E32" t="s">
+        <v>1446</v>
+      </c>
+      <c r="F32" t="s">
         <v>135</v>
       </c>
-      <c r="G7" s="16" t="s">
+      <c r="G32" t="s">
         <v>15</v>
       </c>
-      <c r="H7" s="16">
+      <c r="H32">
         <v>0</v>
       </c>
-      <c r="I7" s="16" t="s">
+      <c r="I32" t="s">
         <v>23</v>
       </c>
-      <c r="J7" s="16" t="s">
-        <v>1415</v>
-      </c>
-      <c r="K7" s="16" t="s">
-        <v>1378</v>
-      </c>
-    </row>
-    <row r="8" spans="1:11">
-      <c r="A8" s="16">
-        <v>17</v>
-      </c>
-      <c r="B8" s="16" t="s">
-        <v>86</v>
-      </c>
-      <c r="C8" s="16" t="s">
-        <v>99</v>
-      </c>
-      <c r="D8" s="16" t="s">
-        <v>100</v>
-      </c>
-      <c r="E8" s="18" t="s">
-        <v>1447</v>
-      </c>
-      <c r="F8" s="16" t="s">
-        <v>1403</v>
-      </c>
-      <c r="G8" s="16" t="s">
+      <c r="K32" s="18" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="33" spans="1:11" ht="15.5">
+      <c r="A33">
+        <v>101</v>
+      </c>
+      <c r="B33" t="s">
+        <v>127</v>
+      </c>
+      <c r="C33" t="s">
+        <v>157</v>
+      </c>
+      <c r="D33" t="s">
+        <v>158</v>
+      </c>
+      <c r="E33" t="s">
+        <v>1459</v>
+      </c>
+      <c r="F33" t="s">
+        <v>135</v>
+      </c>
+      <c r="G33" t="s">
         <v>15</v>
       </c>
-      <c r="H8" s="16">
+      <c r="H33">
         <v>0</v>
       </c>
-      <c r="I8" s="16" t="s">
+      <c r="I33" t="s">
         <v>23</v>
       </c>
-      <c r="J8" s="16" t="s">
-        <v>1407</v>
-      </c>
-      <c r="K8" s="17" t="s">
-        <v>1400</v>
-      </c>
-    </row>
-    <row r="9" spans="1:11">
-      <c r="A9" s="16">
-        <v>23</v>
-      </c>
-      <c r="B9" s="16" t="s">
-        <v>86</v>
-      </c>
-      <c r="C9" s="16" t="s">
-        <v>99</v>
-      </c>
-      <c r="D9" s="16" t="s">
-        <v>101</v>
-      </c>
-      <c r="E9" s="16" t="s">
-        <v>1469</v>
-      </c>
-      <c r="F9" s="16" t="s">
-        <v>1411</v>
-      </c>
-      <c r="G9" s="16" t="s">
-        <v>23</v>
-      </c>
-      <c r="H9" s="16">
-        <v>0</v>
-      </c>
-      <c r="I9" s="16" t="s">
-        <v>23</v>
-      </c>
-      <c r="J9" s="16" t="s">
-        <v>1408</v>
-      </c>
-    </row>
-    <row r="10" spans="1:11">
-      <c r="A10" s="16">
-        <v>106</v>
-      </c>
-      <c r="B10" s="16" t="s">
-        <v>86</v>
-      </c>
-      <c r="C10" s="16" t="s">
-        <v>102</v>
-      </c>
-      <c r="D10" s="16" t="s">
-        <v>103</v>
-      </c>
-      <c r="E10" s="16" t="s">
-        <v>1450</v>
-      </c>
-      <c r="F10" s="16" t="s">
-        <v>135</v>
-      </c>
-      <c r="G10" s="16" t="s">
-        <v>23</v>
-      </c>
-      <c r="H10" s="16" t="s">
-        <v>23</v>
-      </c>
-      <c r="I10" s="16" t="s">
-        <v>23</v>
-      </c>
-      <c r="J10" s="16" t="s">
-        <v>1410</v>
-      </c>
-      <c r="K10" s="16" t="s">
-        <v>1377</v>
-      </c>
-    </row>
-    <row r="11" spans="1:11">
-      <c r="A11" s="16">
-        <v>108</v>
-      </c>
-      <c r="B11" s="16" t="s">
-        <v>86</v>
-      </c>
-      <c r="C11" s="16" t="s">
-        <v>104</v>
-      </c>
-      <c r="D11" s="16" t="s">
-        <v>105</v>
-      </c>
-      <c r="E11" s="16" t="s">
-        <v>1447</v>
-      </c>
-      <c r="F11" s="16" t="s">
-        <v>135</v>
-      </c>
-      <c r="G11" s="16" t="s">
-        <v>15</v>
-      </c>
-      <c r="H11" s="16">
-        <v>0</v>
-      </c>
-      <c r="I11" s="16" t="s">
-        <v>23</v>
-      </c>
-      <c r="J11" s="16" t="s">
-        <v>1406</v>
-      </c>
-      <c r="K11" s="17" t="s">
-        <v>1374</v>
-      </c>
-    </row>
-    <row r="12" spans="1:11">
-      <c r="A12" s="16">
-        <v>110</v>
-      </c>
-      <c r="B12" s="16" t="s">
-        <v>106</v>
-      </c>
-      <c r="C12" s="16" t="s">
-        <v>107</v>
-      </c>
-      <c r="D12" s="16" t="s">
-        <v>108</v>
-      </c>
-      <c r="E12" s="16" t="s">
-        <v>1467</v>
-      </c>
-      <c r="F12" s="16" t="s">
-        <v>135</v>
-      </c>
-      <c r="G12" s="16" t="s">
-        <v>15</v>
-      </c>
-      <c r="H12" s="16">
-        <v>0</v>
-      </c>
-      <c r="I12" s="16" t="s">
-        <v>23</v>
-      </c>
-      <c r="J12" s="16" t="s">
-        <v>1422</v>
-      </c>
-      <c r="K12" s="16" t="s">
-        <v>1073</v>
-      </c>
-    </row>
-    <row r="13" spans="1:11">
-      <c r="A13" s="16">
-        <v>1</v>
-      </c>
-      <c r="B13" s="16" t="s">
-        <v>106</v>
-      </c>
-      <c r="C13" s="16" t="s">
-        <v>109</v>
-      </c>
-      <c r="D13" s="16" t="s">
-        <v>110</v>
-      </c>
-      <c r="F13" s="16" t="s">
-        <v>135</v>
-      </c>
-      <c r="G13" s="16" t="s">
-        <v>15</v>
-      </c>
-      <c r="H13" s="16">
-        <v>0</v>
-      </c>
-      <c r="I13" s="16" t="s">
-        <v>23</v>
-      </c>
-      <c r="K13" s="16" t="s">
-        <v>1379</v>
-      </c>
-    </row>
-    <row r="14" spans="1:11">
-      <c r="A14" s="16">
-        <v>8</v>
-      </c>
-      <c r="B14" s="16" t="s">
-        <v>106</v>
-      </c>
-      <c r="C14" s="16" t="s">
-        <v>111</v>
-      </c>
-      <c r="D14" s="16" t="s">
-        <v>112</v>
-      </c>
-      <c r="E14" s="16" t="s">
-        <v>1459</v>
-      </c>
-      <c r="F14" s="16" t="s">
-        <v>135</v>
-      </c>
-      <c r="G14" s="16" t="s">
-        <v>15</v>
-      </c>
-      <c r="H14" s="16">
-        <v>2</v>
-      </c>
-      <c r="I14" s="16" t="s">
-        <v>145</v>
-      </c>
-      <c r="J14" s="16" t="s">
-        <v>1383</v>
-      </c>
-      <c r="K14" s="16" t="s">
-        <v>1382</v>
-      </c>
-    </row>
-    <row r="15" spans="1:11">
-      <c r="A15" s="16">
-        <v>105</v>
-      </c>
-      <c r="B15" s="16" t="s">
-        <v>106</v>
-      </c>
-      <c r="C15" s="16" t="s">
-        <v>113</v>
-      </c>
-      <c r="D15" s="16" t="s">
-        <v>114</v>
-      </c>
-      <c r="F15" s="16" t="s">
-        <v>135</v>
-      </c>
-      <c r="G15" s="16" t="s">
-        <v>15</v>
-      </c>
-      <c r="H15" s="16">
-        <v>0</v>
-      </c>
-      <c r="I15" s="16" t="s">
-        <v>23</v>
-      </c>
-      <c r="J15" s="16" t="s">
-        <v>1385</v>
-      </c>
-      <c r="K15" s="16" t="s">
-        <v>1384</v>
-      </c>
-    </row>
-    <row r="16" spans="1:11">
-      <c r="A16" s="16">
-        <v>19</v>
-      </c>
-      <c r="B16" s="16" t="s">
-        <v>106</v>
-      </c>
-      <c r="C16" s="16" t="s">
-        <v>115</v>
-      </c>
-      <c r="D16" s="16" t="s">
-        <v>116</v>
-      </c>
-      <c r="F16" s="16" t="s">
-        <v>135</v>
-      </c>
-      <c r="G16" s="16" t="s">
-        <v>15</v>
-      </c>
-      <c r="H16" s="16">
-        <v>2</v>
-      </c>
-      <c r="I16" s="16" t="s">
-        <v>145</v>
-      </c>
-      <c r="J16" s="16" t="s">
-        <v>1387</v>
-      </c>
-      <c r="K16" s="16" t="s">
-        <v>1388</v>
-      </c>
-    </row>
-    <row r="17" spans="1:24">
-      <c r="A17" s="16">
-        <v>25</v>
-      </c>
-      <c r="B17" s="16" t="s">
-        <v>106</v>
-      </c>
-      <c r="C17" s="16" t="s">
-        <v>117</v>
-      </c>
-      <c r="D17" s="16" t="s">
-        <v>118</v>
-      </c>
-      <c r="E17" s="16" t="s">
-        <v>1466</v>
-      </c>
-      <c r="F17" s="16" t="s">
-        <v>135</v>
-      </c>
-      <c r="G17" s="16" t="s">
-        <v>15</v>
-      </c>
-      <c r="H17" s="16">
-        <v>1</v>
-      </c>
-      <c r="I17" s="16" t="s">
-        <v>1390</v>
-      </c>
-      <c r="J17" s="16" t="s">
-        <v>1405</v>
-      </c>
-      <c r="K17" s="16" t="s">
-        <v>1389</v>
-      </c>
-      <c r="X17" s="19" t="s">
-        <v>1404</v>
-      </c>
-    </row>
-    <row r="18" spans="1:24">
-      <c r="A18" s="16">
-        <v>26</v>
-      </c>
-      <c r="B18" s="16" t="s">
-        <v>106</v>
-      </c>
-      <c r="C18" s="16" t="s">
-        <v>119</v>
-      </c>
-      <c r="D18" s="16" t="s">
-        <v>120</v>
-      </c>
-      <c r="F18" s="16" t="s">
-        <v>135</v>
-      </c>
-      <c r="G18" s="16" t="s">
-        <v>15</v>
-      </c>
-      <c r="H18" s="16">
-        <v>0</v>
-      </c>
-      <c r="I18" s="16" t="s">
-        <v>23</v>
-      </c>
-      <c r="K18" s="16" t="s">
-        <v>1391</v>
-      </c>
-    </row>
-    <row r="19" spans="1:24">
-      <c r="A19" s="16">
-        <v>7</v>
-      </c>
-      <c r="B19" s="16" t="s">
-        <v>106</v>
-      </c>
-      <c r="C19" s="16" t="s">
-        <v>121</v>
-      </c>
-      <c r="D19" s="16" t="s">
-        <v>122</v>
-      </c>
-      <c r="F19" s="16" t="s">
-        <v>135</v>
-      </c>
-      <c r="G19" s="16" t="s">
-        <v>15</v>
-      </c>
-      <c r="H19" s="16">
-        <v>1</v>
-      </c>
-      <c r="I19" s="16" t="s">
-        <v>145</v>
-      </c>
-      <c r="J19" s="16" t="s">
-        <v>1392</v>
-      </c>
-      <c r="K19" s="16" t="s">
-        <v>618</v>
-      </c>
-    </row>
-    <row r="20" spans="1:24">
-      <c r="A20" s="16">
-        <v>14</v>
-      </c>
-      <c r="B20" s="16" t="s">
-        <v>106</v>
-      </c>
-      <c r="C20" s="16" t="s">
-        <v>123</v>
-      </c>
-      <c r="D20" s="16" t="s">
-        <v>124</v>
-      </c>
-      <c r="E20" s="16" t="s">
-        <v>1462</v>
-      </c>
-      <c r="F20" s="18" t="s">
-        <v>15</v>
-      </c>
-      <c r="G20" s="16" t="s">
-        <v>15</v>
-      </c>
-      <c r="H20" s="16">
-        <v>0</v>
-      </c>
-      <c r="I20" s="16" t="s">
-        <v>23</v>
-      </c>
-      <c r="J20" s="16" t="s">
-        <v>1423</v>
-      </c>
-      <c r="K20" s="16" t="s">
-        <v>1395</v>
-      </c>
-    </row>
-    <row r="21" spans="1:24" ht="15" customHeight="1">
-      <c r="A21" s="16">
-        <v>22</v>
-      </c>
-      <c r="B21" s="16" t="s">
-        <v>106</v>
-      </c>
-      <c r="C21" s="16" t="s">
-        <v>125</v>
-      </c>
-      <c r="D21" s="16" t="s">
-        <v>126</v>
-      </c>
-      <c r="F21" s="16" t="s">
-        <v>135</v>
-      </c>
-      <c r="G21" s="16" t="s">
-        <v>15</v>
-      </c>
-      <c r="H21" s="16">
-        <v>0</v>
-      </c>
-      <c r="I21" s="16" t="s">
-        <v>23</v>
-      </c>
-      <c r="J21" s="16" t="s">
-        <v>1399</v>
-      </c>
-      <c r="K21" s="16" t="s">
-        <v>1397</v>
-      </c>
-    </row>
-    <row r="22" spans="1:24">
-      <c r="A22" s="16">
-        <v>24</v>
-      </c>
-      <c r="B22" s="16" t="s">
-        <v>127</v>
-      </c>
-      <c r="C22" s="16" t="s">
-        <v>128</v>
-      </c>
-      <c r="D22" s="16" t="s">
-        <v>129</v>
-      </c>
-      <c r="F22" s="16" t="s">
-        <v>135</v>
-      </c>
-      <c r="G22" s="16" t="s">
-        <v>15</v>
-      </c>
-      <c r="H22" s="16">
-        <v>0</v>
-      </c>
-      <c r="I22" s="16" t="s">
-        <v>23</v>
-      </c>
-      <c r="K22" s="16" t="s">
-        <v>1398</v>
-      </c>
-    </row>
-    <row r="23" spans="1:24" ht="15.5">
-      <c r="A23" s="16">
-        <v>27</v>
-      </c>
-      <c r="B23" s="16" t="s">
-        <v>127</v>
-      </c>
-      <c r="C23" s="16" t="s">
-        <v>130</v>
-      </c>
-      <c r="D23" s="16" t="s">
-        <v>131</v>
-      </c>
-      <c r="F23" s="16" t="s">
-        <v>135</v>
-      </c>
-      <c r="G23" s="16" t="s">
-        <v>15</v>
-      </c>
-      <c r="H23" s="16">
-        <v>0</v>
-      </c>
-      <c r="I23" s="16" t="s">
-        <v>23</v>
-      </c>
-      <c r="K23" s="20" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="24" spans="1:24">
-      <c r="A24" s="16">
-        <v>28</v>
-      </c>
-      <c r="B24" s="16" t="s">
-        <v>127</v>
-      </c>
-      <c r="C24" s="16" t="s">
-        <v>133</v>
-      </c>
-      <c r="D24" s="16" t="s">
-        <v>134</v>
-      </c>
-      <c r="E24" s="16" t="s">
-        <v>1468</v>
-      </c>
-      <c r="F24" s="16" t="s">
-        <v>135</v>
-      </c>
-      <c r="G24" s="16" t="s">
-        <v>15</v>
-      </c>
-      <c r="H24" s="16">
-        <v>0</v>
-      </c>
-      <c r="I24" s="16" t="s">
-        <v>23</v>
-      </c>
-      <c r="J24" s="16" t="s">
-        <v>1386</v>
-      </c>
-      <c r="K24" s="17" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="25" spans="1:24">
-      <c r="A25" s="16">
-        <v>28</v>
-      </c>
-      <c r="B25" s="16" t="s">
-        <v>127</v>
-      </c>
-      <c r="C25" s="16" t="s">
-        <v>138</v>
-      </c>
-      <c r="D25" s="16" t="s">
-        <v>134</v>
-      </c>
-      <c r="E25" s="16" t="s">
-        <v>1468</v>
-      </c>
-      <c r="F25" s="16" t="s">
-        <v>135</v>
-      </c>
-      <c r="G25" s="16" t="s">
-        <v>15</v>
-      </c>
-      <c r="H25" s="16">
-        <v>0</v>
-      </c>
-      <c r="I25" s="16" t="s">
-        <v>23</v>
-      </c>
-      <c r="J25" s="16" t="s">
-        <v>1386</v>
-      </c>
-      <c r="K25" s="17" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="26" spans="1:24" ht="15.5">
-      <c r="A26" s="16">
-        <v>102</v>
-      </c>
-      <c r="B26" s="16" t="s">
-        <v>127</v>
-      </c>
-      <c r="C26" s="16" t="s">
-        <v>139</v>
-      </c>
-      <c r="D26" s="16" t="s">
-        <v>140</v>
-      </c>
-      <c r="E26" s="16" t="s">
-        <v>1461</v>
-      </c>
-      <c r="F26" s="16" t="s">
-        <v>135</v>
-      </c>
-      <c r="G26" s="16" t="s">
-        <v>15</v>
-      </c>
-      <c r="H26" s="16">
-        <v>0</v>
-      </c>
-      <c r="I26" s="16" t="s">
-        <v>23</v>
-      </c>
-      <c r="J26" s="16" t="s">
-        <v>142</v>
-      </c>
-      <c r="K26" s="21" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="27" spans="1:24" ht="15.5">
-      <c r="A27" s="16">
-        <v>111</v>
-      </c>
-      <c r="B27" s="16" t="s">
-        <v>127</v>
-      </c>
-      <c r="C27" s="16" t="s">
-        <v>143</v>
-      </c>
-      <c r="D27" s="16" t="s">
-        <v>144</v>
-      </c>
-      <c r="E27" s="16" t="s">
-        <v>1447</v>
-      </c>
-      <c r="F27" s="16" t="s">
-        <v>135</v>
-      </c>
-      <c r="G27" s="16" t="s">
-        <v>135</v>
-      </c>
-      <c r="H27" s="16">
-        <v>1</v>
-      </c>
-      <c r="I27" s="16" t="s">
-        <v>145</v>
-      </c>
-      <c r="J27" s="16" t="s">
-        <v>147</v>
-      </c>
-      <c r="K27" s="21" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="28" spans="1:24" ht="15.5">
-      <c r="A28" s="16">
-        <v>112</v>
-      </c>
-      <c r="B28" s="16" t="s">
-        <v>127</v>
-      </c>
-      <c r="C28" s="16" t="s">
-        <v>148</v>
-      </c>
-      <c r="D28" s="16" t="s">
-        <v>96</v>
-      </c>
-      <c r="E28" s="16" t="s">
-        <v>1459</v>
-      </c>
-      <c r="F28" s="16" t="s">
-        <v>135</v>
-      </c>
-      <c r="G28" s="16" t="s">
-        <v>1421</v>
-      </c>
-      <c r="H28" s="16">
-        <v>1</v>
-      </c>
-      <c r="I28" s="16" t="s">
-        <v>136</v>
-      </c>
-      <c r="K28" s="21" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="29" spans="1:24">
-      <c r="A29" s="16">
-        <v>113</v>
-      </c>
-      <c r="B29" s="16" t="s">
-        <v>127</v>
-      </c>
-      <c r="C29" s="16" t="s">
-        <v>150</v>
-      </c>
-      <c r="D29" s="16" t="s">
-        <v>151</v>
-      </c>
-      <c r="E29" s="16" t="s">
-        <v>1459</v>
-      </c>
-      <c r="F29" s="16" t="s">
-        <v>135</v>
-      </c>
-      <c r="G29" s="16" t="s">
-        <v>135</v>
-      </c>
-      <c r="H29" s="16">
-        <v>1</v>
-      </c>
-      <c r="I29" s="16" t="s">
-        <v>145</v>
-      </c>
-      <c r="K29" s="16" t="s">
-        <v>1396</v>
-      </c>
-    </row>
-    <row r="30" spans="1:24">
-      <c r="A30" s="16">
-        <v>113</v>
-      </c>
-      <c r="B30" s="16" t="s">
-        <v>127</v>
-      </c>
-      <c r="C30" s="16" t="s">
-        <v>150</v>
-      </c>
-      <c r="D30" s="16" t="s">
-        <v>151</v>
-      </c>
-      <c r="E30" s="16" t="s">
-        <v>1459</v>
-      </c>
-      <c r="F30" s="16" t="s">
-        <v>1418</v>
-      </c>
-      <c r="G30" s="16" t="s">
-        <v>135</v>
-      </c>
-      <c r="H30" s="16">
-        <v>4</v>
-      </c>
-      <c r="I30" s="16" t="s">
-        <v>145</v>
-      </c>
-      <c r="K30" s="16" t="s">
-        <v>1396</v>
-      </c>
-    </row>
-    <row r="31" spans="1:24" ht="15.5">
-      <c r="A31" s="16">
-        <v>104</v>
-      </c>
-      <c r="B31" s="16" t="s">
-        <v>127</v>
-      </c>
-      <c r="C31" s="16" t="s">
-        <v>152</v>
-      </c>
-      <c r="D31" s="16" t="s">
-        <v>103</v>
-      </c>
-      <c r="E31" s="16" t="s">
-        <v>1460</v>
-      </c>
-      <c r="F31" s="16" t="s">
-        <v>135</v>
-      </c>
-      <c r="G31" s="16" t="s">
-        <v>15</v>
-      </c>
-      <c r="H31" s="16">
-        <v>0</v>
-      </c>
-      <c r="I31" s="16" t="s">
-        <v>23</v>
-      </c>
-      <c r="K31" s="21" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="32" spans="1:24" ht="15.5">
-      <c r="A32" s="16">
-        <v>107</v>
-      </c>
-      <c r="B32" s="16" t="s">
-        <v>127</v>
-      </c>
-      <c r="C32" s="16" t="s">
-        <v>154</v>
-      </c>
-      <c r="D32" s="16" t="s">
-        <v>155</v>
-      </c>
-      <c r="E32" s="16" t="s">
-        <v>1447</v>
-      </c>
-      <c r="F32" s="16" t="s">
-        <v>135</v>
-      </c>
-      <c r="G32" s="16" t="s">
-        <v>15</v>
-      </c>
-      <c r="H32" s="16">
-        <v>0</v>
-      </c>
-      <c r="I32" s="16" t="s">
-        <v>23</v>
-      </c>
-      <c r="K32" s="21" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="33" spans="1:11" ht="15.5">
-      <c r="A33" s="16">
-        <v>101</v>
-      </c>
-      <c r="B33" s="16" t="s">
-        <v>127</v>
-      </c>
-      <c r="C33" s="16" t="s">
-        <v>157</v>
-      </c>
-      <c r="D33" s="16" t="s">
-        <v>158</v>
-      </c>
-      <c r="E33" s="16" t="s">
-        <v>1460</v>
-      </c>
-      <c r="F33" s="16" t="s">
-        <v>135</v>
-      </c>
-      <c r="G33" s="16" t="s">
-        <v>15</v>
-      </c>
-      <c r="H33" s="16">
-        <v>0</v>
-      </c>
-      <c r="I33" s="16" t="s">
-        <v>23</v>
-      </c>
-      <c r="J33" s="16" t="s">
+      <c r="J33" t="s">
         <v>1394</v>
       </c>
-      <c r="K33" s="21" t="s">
+      <c r="K33" s="18" t="s">
         <v>1393</v>
       </c>
     </row>
@@ -12039,11 +12034,11 @@
       <c r="AE3" s="3"/>
     </row>
     <row r="4" spans="1:31">
-      <c r="A4" s="15" t="s">
+      <c r="A4" s="19" t="s">
         <v>181</v>
       </c>
-      <c r="B4" s="15"/>
-      <c r="C4" s="15"/>
+      <c r="B4" s="19"/>
+      <c r="C4" s="19"/>
       <c r="D4" s="5">
         <v>33284114</v>
       </c>
@@ -12533,11 +12528,11 @@
       <c r="AE13" s="3"/>
     </row>
     <row r="14" spans="1:31">
-      <c r="A14" s="15" t="s">
+      <c r="A14" s="19" t="s">
         <v>181</v>
       </c>
-      <c r="B14" s="15"/>
-      <c r="C14" s="15"/>
+      <c r="B14" s="19"/>
+      <c r="C14" s="19"/>
       <c r="D14" s="5">
         <v>33230550</v>
       </c>
@@ -12974,11 +12969,11 @@
       <c r="AE22" s="3"/>
     </row>
     <row r="23" spans="1:31">
-      <c r="A23" s="15" t="s">
+      <c r="A23" s="19" t="s">
         <v>256</v>
       </c>
-      <c r="B23" s="15"/>
-      <c r="C23" s="15"/>
+      <c r="B23" s="19"/>
+      <c r="C23" s="19"/>
       <c r="D23" s="5">
         <v>35344464</v>
       </c>
@@ -13147,19 +13142,19 @@
       <c r="L26" s="2"/>
       <c r="M26" s="2"/>
       <c r="N26" s="2"/>
-      <c r="O26" s="15"/>
-      <c r="P26" s="15"/>
+      <c r="O26" s="19"/>
+      <c r="P26" s="19"/>
       <c r="Q26" s="2"/>
       <c r="R26" s="2"/>
       <c r="S26" s="2"/>
       <c r="T26" s="2"/>
-      <c r="U26" s="15"/>
-      <c r="V26" s="15"/>
+      <c r="U26" s="19"/>
+      <c r="V26" s="19"/>
       <c r="W26" s="2"/>
       <c r="X26" s="2"/>
       <c r="Y26" s="2"/>
-      <c r="Z26" s="15"/>
-      <c r="AA26" s="15"/>
+      <c r="Z26" s="19"/>
+      <c r="AA26" s="19"/>
       <c r="AB26" s="2"/>
       <c r="AC26" s="2"/>
       <c r="AD26" s="2"/>
@@ -13601,8 +13596,8 @@
       <c r="S35" s="3"/>
       <c r="T35" s="3"/>
       <c r="U35" s="2"/>
-      <c r="V35" s="15"/>
-      <c r="W35" s="15"/>
+      <c r="V35" s="19"/>
+      <c r="W35" s="19"/>
       <c r="X35" s="3"/>
       <c r="Y35" s="3"/>
       <c r="Z35" s="3"/>

</xml_diff>